<commit_message>
Fixed Outlier symbol in Multi Excel
Changed outlier to !
</commit_message>
<xml_diff>
--- a/excel/MultiAnalytesMU.xlsx
+++ b/excel/MultiAnalytesMU.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="38" windowWidth="15960" windowHeight="18083"/>
+    <workbookView xWindow="0" yWindow="38" windowWidth="15960" windowHeight="18083" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="MainTable" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="108">
   <si>
     <r>
       <rPr>
@@ -1408,6 +1408,9 @@
       </rPr>
       <t>Corrected for Recovery with Uncertainty</t>
     </r>
+  </si>
+  <si>
+    <t>!58.97</t>
   </si>
 </sst>
 </file>
@@ -2985,27 +2988,6 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="20" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="20" fillId="5" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="63" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
@@ -3104,22 +3086,10 @@
       <alignment horizontal="right" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="11" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -3133,86 +3103,119 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="13" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="12" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="49" fontId="20" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="5" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="102">
+  <dxfs count="37">
     <dxf>
       <font>
         <color theme="1"/>
@@ -3548,584 +3551,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFD38A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9781"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF932092"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="16"/>
-          <bgColor indexed="42"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF932092"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="16"/>
-          <bgColor indexed="19"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="16"/>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="16"/>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFA7A7A7"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="16"/>
-          <bgColor indexed="31"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFA5A5A5"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="16"/>
-          <bgColor indexed="31"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFA5A5A5"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF929292"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFFFF"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="16"/>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="16"/>
-          <bgColor indexed="28"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="16"/>
-          <bgColor indexed="32"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="16"/>
-          <bgColor indexed="28"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="16"/>
-          <bgColor indexed="31"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFDDDDDD"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="16"/>
-          <bgColor indexed="29"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="16"/>
-          <bgColor indexed="28"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="16"/>
-          <bgColor indexed="26"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFDDDDDD"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFDDDDDD"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="16"/>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF0432FF"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="16"/>
-          <bgColor indexed="25"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF929292"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="16"/>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF929292"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF707070"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="16"/>
-          <bgColor indexed="19"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FF0432FF"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="16"/>
-          <bgColor indexed="17"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFD38A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9781"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF932092"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="16"/>
-          <bgColor indexed="42"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF932092"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="16"/>
-          <bgColor indexed="19"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="16"/>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="16"/>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFA7A7A7"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="16"/>
-          <bgColor indexed="31"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFA5A5A5"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="16"/>
-          <bgColor indexed="31"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFA5A5A5"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF929292"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFFFF"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="16"/>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="16"/>
-          <bgColor indexed="28"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="16"/>
-          <bgColor indexed="32"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="16"/>
-          <bgColor indexed="28"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="16"/>
-          <bgColor indexed="31"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFDDDDDD"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="16"/>
-          <bgColor indexed="29"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="16"/>
-          <bgColor indexed="28"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="16"/>
-          <bgColor indexed="26"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFDDDDDD"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFDDDDDD"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="16"/>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="16"/>
-          <bgColor indexed="26"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF0432FF"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="16"/>
-          <bgColor indexed="25"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF929292"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="16"/>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF929292"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF707070"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="16"/>
-          <bgColor indexed="19"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FF0432FF"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="16"/>
-          <bgColor indexed="17"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0"/>
   <colors>
@@ -4297,7 +3722,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{C572A759-6A51-4108-AA02-DFA0A04FC94B}">
-            <ma14:wrappingTextBoxFlag xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" val="1"/>
+            <ma14:wrappingTextBoxFlag xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" val="1"/>
           </a:ext>
         </a:extLst>
       </xdr:spPr>
@@ -4843,7 +4268,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{C572A759-6A51-4108-AA02-DFA0A04FC94B}">
-            <ma14:wrappingTextBoxFlag xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" val="1"/>
+            <ma14:wrappingTextBoxFlag xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" val="1"/>
           </a:ext>
         </a:extLst>
       </xdr:spPr>
@@ -5985,25 +5410,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AA53"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.1" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="4.125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="35.25" style="154" customWidth="1"/>
-    <col min="3" max="3" width="14.9375" style="154" customWidth="1"/>
+    <col min="2" max="2" width="35.25" style="143" customWidth="1"/>
+    <col min="3" max="3" width="14.9375" style="143" customWidth="1"/>
     <col min="4" max="27" width="21.375" style="1" customWidth="1"/>
     <col min="28" max="28" width="8.875" style="1" customWidth="1"/>
     <col min="29" max="16384" width="8.875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:27" ht="20.55" customHeight="1">
-      <c r="B1" s="149" t="s">
+      <c r="B1" s="173" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="155"/>
+      <c r="C1" s="174"/>
       <c r="D1" s="2" t="str">
         <f>IF(ISTEXT(SampleResults!$A$1),SampleResults!$A$1,"TestName")</f>
         <v>ICP-MS</v>
@@ -6102,10 +5527,10 @@
       </c>
     </row>
     <row r="2" spans="2:27" ht="20.55" customHeight="1">
-      <c r="B2" s="150" t="s">
+      <c r="B2" s="175" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="156"/>
+      <c r="C2" s="176"/>
       <c r="D2" s="3" t="str">
         <f>SampleResults!B1</f>
         <v>Al</v>
@@ -6204,10 +5629,10 @@
       </c>
     </row>
     <row r="3" spans="2:27" ht="14.25" customHeight="1">
-      <c r="B3" s="151" t="s">
+      <c r="B3" s="140" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="152" t="s">
+      <c r="C3" s="141" t="s">
         <v>3</v>
       </c>
       <c r="D3" s="4" t="str">
@@ -6311,7 +5736,7 @@
       <c r="B4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="140" t="s">
+      <c r="C4" s="133" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="7" t="str">
@@ -6415,7 +5840,7 @@
       <c r="B5" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="141">
+      <c r="C5" s="134">
         <v>2</v>
       </c>
       <c r="D5" s="10">
@@ -6515,124 +5940,124 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:27" s="128" customFormat="1" ht="17.95" customHeight="1">
-      <c r="B6" s="145" t="s">
+    <row r="6" spans="2:27" s="121" customFormat="1" ht="17.95" customHeight="1">
+      <c r="B6" s="156" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="157"/>
-      <c r="D6" s="142">
+      <c r="D6" s="135">
         <v>90</v>
       </c>
-      <c r="E6" s="142">
+      <c r="E6" s="135">
         <v>2.2000000000000002</v>
       </c>
-      <c r="F6" s="142">
+      <c r="F6" s="135">
         <v>99</v>
       </c>
-      <c r="G6" s="142">
+      <c r="G6" s="135">
         <v>90</v>
       </c>
-      <c r="H6" s="142">
+      <c r="H6" s="135">
         <v>92</v>
       </c>
-      <c r="I6" s="142">
+      <c r="I6" s="135">
         <v>9</v>
       </c>
-      <c r="J6" s="142">
+      <c r="J6" s="135">
         <v>95</v>
       </c>
-      <c r="K6" s="142">
+      <c r="K6" s="135">
         <v>90</v>
       </c>
-      <c r="L6" s="142">
+      <c r="L6" s="135">
         <v>90</v>
       </c>
-      <c r="M6" s="142">
+      <c r="M6" s="135">
         <v>90</v>
       </c>
-      <c r="N6" s="142">
+      <c r="N6" s="135">
         <v>1</v>
       </c>
-      <c r="O6" s="142">
+      <c r="O6" s="135">
         <v>90</v>
       </c>
-      <c r="P6" s="142">
+      <c r="P6" s="135">
         <v>102</v>
       </c>
-      <c r="Q6" s="142">
+      <c r="Q6" s="135">
         <v>99</v>
       </c>
-      <c r="R6" s="142">
+      <c r="R6" s="135">
         <v>90</v>
       </c>
-      <c r="S6" s="142">
+      <c r="S6" s="135">
         <v>93</v>
       </c>
-      <c r="T6" s="142">
+      <c r="T6" s="135">
         <v>108</v>
       </c>
-      <c r="U6" s="142">
+      <c r="U6" s="135">
         <v>90</v>
       </c>
-      <c r="V6" s="142">
+      <c r="V6" s="135">
         <v>1.01E-3</v>
       </c>
-      <c r="W6" s="142">
+      <c r="W6" s="135">
         <v>106</v>
       </c>
-      <c r="X6" s="142">
+      <c r="X6" s="135">
         <v>1.155</v>
       </c>
-      <c r="Y6" s="142">
+      <c r="Y6" s="135">
         <v>0.11550000000000001</v>
       </c>
-      <c r="Z6" s="142">
+      <c r="Z6" s="135">
         <v>1.155E-2</v>
       </c>
-      <c r="AA6" s="142">
+      <c r="AA6" s="135">
         <v>1151</v>
       </c>
     </row>
-    <row r="7" spans="2:27" s="128" customFormat="1" ht="17.95" customHeight="1">
-      <c r="B7" s="146" t="s">
+    <row r="7" spans="2:27" s="121" customFormat="1" ht="17.95" customHeight="1">
+      <c r="B7" s="158" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="158"/>
-      <c r="D7" s="143"/>
-      <c r="E7" s="143"/>
-      <c r="F7" s="143"/>
-      <c r="G7" s="143"/>
-      <c r="H7" s="143"/>
-      <c r="I7" s="143"/>
-      <c r="J7" s="143"/>
-      <c r="K7" s="143"/>
-      <c r="L7" s="143"/>
-      <c r="M7" s="144">
+      <c r="C7" s="159"/>
+      <c r="D7" s="136"/>
+      <c r="E7" s="136"/>
+      <c r="F7" s="136"/>
+      <c r="G7" s="136"/>
+      <c r="H7" s="136"/>
+      <c r="I7" s="136"/>
+      <c r="J7" s="136"/>
+      <c r="K7" s="136"/>
+      <c r="L7" s="136"/>
+      <c r="M7" s="137">
         <v>1</v>
       </c>
-      <c r="N7" s="143"/>
-      <c r="O7" s="143"/>
-      <c r="P7" s="143"/>
-      <c r="Q7" s="143"/>
-      <c r="R7" s="143"/>
-      <c r="S7" s="143"/>
-      <c r="T7" s="143"/>
-      <c r="U7" s="143"/>
-      <c r="V7" s="143"/>
-      <c r="W7" s="143"/>
-      <c r="X7" s="143"/>
-      <c r="Y7" s="143"/>
-      <c r="Z7" s="143"/>
-      <c r="AA7" s="143"/>
+      <c r="N7" s="136"/>
+      <c r="O7" s="136"/>
+      <c r="P7" s="136"/>
+      <c r="Q7" s="136"/>
+      <c r="R7" s="136"/>
+      <c r="S7" s="136"/>
+      <c r="T7" s="136"/>
+      <c r="U7" s="136"/>
+      <c r="V7" s="136"/>
+      <c r="W7" s="136"/>
+      <c r="X7" s="136"/>
+      <c r="Y7" s="136"/>
+      <c r="Z7" s="136"/>
+      <c r="AA7" s="136"/>
     </row>
     <row r="8" spans="2:27" ht="16.899999999999999" customHeight="1">
-      <c r="B8" s="159" t="s">
+      <c r="B8" s="168" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="160"/>
-      <c r="D8" s="11">
+      <c r="C8" s="163"/>
+      <c r="D8" s="11" t="str">
         <f t="shared" ref="D8:AA8" si="4">IF(D38&gt;0,D25+D38&amp;" ("&amp;D38&amp;" Excluded!)",D25)</f>
-        <v>9</v>
+        <v>9 (1 Excluded!)</v>
       </c>
       <c r="E8" s="12">
         <f t="shared" si="4"/>
@@ -6728,13 +6153,13 @@
       </c>
     </row>
     <row r="9" spans="2:27" ht="16.899999999999999" customHeight="1">
-      <c r="B9" s="161" t="s">
+      <c r="B9" s="169" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="162"/>
+      <c r="C9" s="165"/>
       <c r="D9" s="13">
         <f t="shared" ref="D9:AA9" si="5">IF(D25&gt;0,D27/D26,0)</f>
-        <v>0.12465678855305257</v>
+        <v>7.6682302939923758E-2</v>
       </c>
       <c r="E9" s="13">
         <f t="shared" si="5"/>
@@ -6830,13 +6255,13 @@
       </c>
     </row>
     <row r="10" spans="2:27" ht="16.899999999999999" customHeight="1">
-      <c r="B10" s="163" t="s">
+      <c r="B10" s="170" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="164"/>
+      <c r="C10" s="167"/>
       <c r="D10" s="14">
         <f t="shared" ref="D10:AA10" si="6">IFERROR(IF(D3="Blank",0,(1-D16)),0)</f>
-        <v>0.10579012345679017</v>
+        <v>7.5916666666666743E-2</v>
       </c>
       <c r="E10" s="14">
         <f t="shared" si="6"/>
@@ -6932,14 +6357,14 @@
       </c>
     </row>
     <row r="11" spans="2:27" ht="16.899999999999999" customHeight="1">
-      <c r="B11" s="116" t="str">
+      <c r="B11" s="171" t="str">
         <f>"Horwitz Ratio (Ideally 0.3≤HorRat≤1) "&amp;IF(COUNTIFS(D11:AA11,"&gt;2")," Check: Very High",IF(COUNTIFS(D11:AA11,"&gt;1"),"Check: High",IF(COUNTIFS(D11:AA11,"&lt;0.3"),"Check: Low?","- OK")))</f>
         <v>Horwitz Ratio (Ideally 0.3≤HorRat≤1)  Check: Very High</v>
       </c>
-      <c r="C11" s="165"/>
+      <c r="C11" s="172"/>
       <c r="D11" s="109">
         <f>((D9*100)/D30)</f>
-        <v>0.56662176615023896</v>
+        <v>0.34855592245419892</v>
       </c>
       <c r="E11" s="15">
         <f t="shared" ref="E11:AA11" si="7">((E9*100)/E30)</f>
@@ -7035,14 +6460,14 @@
       </c>
     </row>
     <row r="12" spans="2:27" ht="16.899999999999999" customHeight="1">
-      <c r="B12" s="166" t="str">
+      <c r="B12" s="154" t="str">
         <f>IF(COUNTIFS(D12:AA12,"&gt;0")," Grubbs' Outlier Check : "&amp;COUNTIFS(D12:AA12,"&gt;0")&amp;" Found?"," Grubbs' Outlier Check")</f>
-        <v xml:space="preserve"> Grubbs' Outlier Check : 4 Found?</v>
-      </c>
-      <c r="C12" s="167"/>
+        <v xml:space="preserve"> Grubbs' Outlier Check : 3 Found?</v>
+      </c>
+      <c r="C12" s="155"/>
       <c r="D12" s="16">
         <f t="shared" ref="D12:AA12" si="8">IFERROR(IF(D34&lt;D36,IF(D35&lt;D36,0,D19),D20),0)</f>
-        <v>58.97</v>
+        <v>0</v>
       </c>
       <c r="E12" s="16">
         <f t="shared" si="8"/>
@@ -7138,14 +6563,14 @@
       </c>
     </row>
     <row r="13" spans="2:27" ht="16.899999999999999" customHeight="1">
-      <c r="B13" s="168" t="str">
+      <c r="B13" s="162" t="str">
         <f>" Result to "&amp;D5&amp;" Significant figures"</f>
         <v xml:space="preserve"> Result to 2 Significant figures</v>
       </c>
-      <c r="C13" s="160"/>
+      <c r="C13" s="163"/>
       <c r="D13" s="17" t="str">
         <f t="shared" ref="D13:AA13" si="9">IFERROR(FIXED(D26,((-1*INT(LOG10(D26)))-1)+D5,TRUE),0)</f>
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="E13" s="17" t="str">
         <f t="shared" si="9"/>
@@ -7241,13 +6666,13 @@
       </c>
     </row>
     <row r="14" spans="2:27" ht="16.899999999999999" customHeight="1">
-      <c r="B14" s="169" t="s">
+      <c r="B14" s="164" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="162"/>
+      <c r="C14" s="165"/>
       <c r="D14" s="18" t="str">
         <f t="shared" ref="D14:AA14" si="10">IFERROR(IF(D3="Blank",0,D51),0)</f>
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="E14" s="18" t="str">
         <f t="shared" si="10"/>
@@ -7343,13 +6768,13 @@
       </c>
     </row>
     <row r="15" spans="2:27" ht="16.899999999999999" customHeight="1">
-      <c r="B15" s="169" t="s">
+      <c r="B15" s="164" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="162"/>
+      <c r="C15" s="165"/>
       <c r="D15" s="18" t="str">
         <f t="shared" ref="D15:AA15" si="11">IFERROR(IF(D3="Blank",0,D45),0)</f>
-        <v>97</v>
+        <v>62</v>
       </c>
       <c r="E15" s="18" t="str">
         <f t="shared" si="11"/>
@@ -7445,13 +6870,13 @@
       </c>
     </row>
     <row r="16" spans="2:27" ht="16.899999999999999" customHeight="1">
-      <c r="B16" s="170" t="s">
+      <c r="B16" s="166" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="164"/>
+      <c r="C16" s="167"/>
       <c r="D16" s="19">
         <f t="shared" ref="D16:AA16" si="12">IFERROR(IF(D3="Blank","Blank",(D26)/D6),0)</f>
-        <v>0.89420987654320983</v>
+        <v>0.92408333333333326</v>
       </c>
       <c r="E16" s="19">
         <f t="shared" si="12"/>
@@ -7547,8 +6972,8 @@
       </c>
     </row>
     <row r="17" spans="2:27" ht="16.899999999999999" hidden="1" customHeight="1">
-      <c r="B17" s="112"/>
-      <c r="C17" s="171"/>
+      <c r="B17" s="177"/>
+      <c r="C17" s="153"/>
       <c r="D17" s="20"/>
       <c r="E17" s="20"/>
       <c r="F17" s="20"/>
@@ -7578,10 +7003,10 @@
       <c r="B18" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="172"/>
+      <c r="C18" s="144"/>
       <c r="D18" s="22">
         <f t="shared" ref="D18:AA18" si="13">IFERROR(IF(D34&lt;D36,IF(D35&lt;D36,0,D19),D20),0)</f>
-        <v>58.97</v>
+        <v>0</v>
       </c>
       <c r="E18" s="22">
         <f t="shared" si="13"/>
@@ -7677,11 +7102,11 @@
       </c>
     </row>
     <row r="19" spans="2:27" ht="18.3" hidden="1" customHeight="1">
-      <c r="B19" s="153" t="str">
+      <c r="B19" s="142" t="str">
         <f>IF(D19=D18,"Ymax (Maximum Value) may be an Outlier!","Ymax (Maximum Value)")</f>
         <v>Ymax (Maximum Value)</v>
       </c>
-      <c r="C19" s="173"/>
+      <c r="C19" s="145"/>
       <c r="D19" s="23">
         <f>MAX(SampleResults!B1:B32)</f>
         <v>89.84</v>
@@ -7780,14 +7205,14 @@
       </c>
     </row>
     <row r="20" spans="2:27" ht="9" hidden="1" customHeight="1">
-      <c r="B20" s="153" t="str">
+      <c r="B20" s="142" t="str">
         <f>IF(D20=D18,"Ymin (Minimum Value) Outlier?","Ymin (Minimum Value)")</f>
-        <v>Ymin (Minimum Value) Outlier?</v>
-      </c>
-      <c r="C20" s="173"/>
+        <v>Ymin (Minimum Value)</v>
+      </c>
+      <c r="C20" s="145"/>
       <c r="D20" s="23">
         <f>MIN(SampleResults!B1:B32)</f>
-        <v>58.97</v>
+        <v>72.11</v>
       </c>
       <c r="E20" s="23">
         <f>MIN(SampleResults!C1:C32)</f>
@@ -7883,8 +7308,8 @@
       </c>
     </row>
     <row r="21" spans="2:27" ht="16.899999999999999" hidden="1" customHeight="1">
-      <c r="B21" s="113"/>
-      <c r="C21" s="171"/>
+      <c r="B21" s="161"/>
+      <c r="C21" s="153"/>
       <c r="D21" s="24"/>
       <c r="E21" s="24"/>
       <c r="F21" s="24"/>
@@ -7911,8 +7336,8 @@
       <c r="AA21" s="24"/>
     </row>
     <row r="22" spans="2:27" ht="16.899999999999999" hidden="1" customHeight="1">
-      <c r="B22" s="113"/>
-      <c r="C22" s="171"/>
+      <c r="B22" s="161"/>
+      <c r="C22" s="153"/>
       <c r="D22" s="24"/>
       <c r="E22" s="24"/>
       <c r="F22" s="24"/>
@@ -7939,8 +7364,8 @@
       <c r="AA22" s="24"/>
     </row>
     <row r="23" spans="2:27" ht="16.899999999999999" hidden="1" customHeight="1">
-      <c r="B23" s="113"/>
-      <c r="C23" s="171"/>
+      <c r="B23" s="161"/>
+      <c r="C23" s="153"/>
       <c r="D23" s="24"/>
       <c r="E23" s="24"/>
       <c r="F23" s="24"/>
@@ -7967,10 +7392,10 @@
       <c r="AA23" s="24"/>
     </row>
     <row r="24" spans="2:27" ht="16.899999999999999" hidden="1" customHeight="1">
-      <c r="B24" s="115" t="s">
+      <c r="B24" s="160" t="s">
         <v>16</v>
       </c>
-      <c r="C24" s="171"/>
+      <c r="C24" s="153"/>
       <c r="D24" s="25" t="str">
         <f t="shared" ref="D24:AA24" si="14">IFERROR(IF(D3="Blank","Blank",D46),0)</f>
         <v>90</v>
@@ -8069,13 +7494,13 @@
       </c>
     </row>
     <row r="25" spans="2:27" ht="16.899999999999999" hidden="1" customHeight="1">
-      <c r="B25" s="174" t="s">
+      <c r="B25" s="146" t="s">
         <v>17</v>
       </c>
-      <c r="C25" s="173"/>
+      <c r="C25" s="145"/>
       <c r="D25" s="23">
         <f>COUNT(SampleResults!B1:B32)</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E25" s="23">
         <f>COUNT(SampleResults!C1:C32)</f>
@@ -8174,10 +7599,10 @@
       <c r="B26" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="C26" s="173"/>
+      <c r="C26" s="145"/>
       <c r="D26" s="26">
         <f>IF(D25&gt;0,AVERAGE(SampleResults!B1:B32),0)</f>
-        <v>80.478888888888889</v>
+        <v>83.16749999999999</v>
       </c>
       <c r="E26" s="26">
         <f>IF(E25&gt;0,AVERAGE(SampleResults!C1:C32),0)</f>
@@ -8276,10 +7701,10 @@
       <c r="B27" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="C27" s="173"/>
+      <c r="C27" s="145"/>
       <c r="D27" s="27">
         <f>IF(D25&gt;1,STDEV(SampleResults!B1:B32),0)</f>
-        <v>10.032239835206834</v>
+        <v>6.3774754297561085</v>
       </c>
       <c r="E27" s="28">
         <f>IF(E25&gt;1,STDEV(SampleResults!C1:C32),0)</f>
@@ -8378,10 +7803,10 @@
       <c r="B28" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="C28" s="173"/>
+      <c r="C28" s="145"/>
       <c r="D28" s="23">
         <f>VLOOKUP(D25-1,Distributions!$A$3:$B$40,2,TRUE)</f>
-        <v>2.8959999999999999</v>
+        <v>2.9980000000000002</v>
       </c>
       <c r="E28" s="23">
         <f>VLOOKUP(E25-1,Distributions!$A$3:$B$40,2,TRUE)</f>
@@ -8480,7 +7905,7 @@
       <c r="B29" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="C29" s="173"/>
+      <c r="C29" s="145"/>
       <c r="D29" s="29">
         <f>VLOOKUP(D4,Units!$A$1:$B$14,2,FALSE)</f>
         <v>1000000000</v>
@@ -8582,7 +8007,7 @@
       <c r="B30" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="C30" s="173"/>
+      <c r="C30" s="145"/>
       <c r="D30" s="30">
         <f t="shared" ref="D30:AA30" si="15">IF(D6/D29&lt;1.2*0.0000001,22,IF(D6/D29&lt;=0.138,2*POWER(D6/D29,-0.15),POWER(D6/D29,-0.5)))</f>
         <v>22</v>
@@ -8681,13 +8106,13 @@
       </c>
     </row>
     <row r="31" spans="2:27" ht="16.899999999999999" hidden="1" customHeight="1">
-      <c r="B31" s="153" t="s">
+      <c r="B31" s="142" t="s">
         <v>23</v>
       </c>
-      <c r="C31" s="175"/>
+      <c r="C31" s="147"/>
       <c r="D31" s="31">
         <f t="shared" ref="D31:AA31" si="16">D19-D26</f>
-        <v>9.3611111111111143</v>
+        <v>6.6725000000000136</v>
       </c>
       <c r="E31" s="31">
         <f t="shared" si="16"/>
@@ -8786,10 +8211,10 @@
       <c r="B32" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="C32" s="173"/>
+      <c r="C32" s="145"/>
       <c r="D32" s="32">
         <f t="shared" ref="D32:AA32" si="17">D26-D20</f>
-        <v>21.50888888888889</v>
+        <v>11.05749999999999</v>
       </c>
       <c r="E32" s="32">
         <f t="shared" si="17"/>
@@ -8888,10 +8313,10 @@
       <c r="B33" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="C33" s="172"/>
+      <c r="C33" s="144"/>
       <c r="D33" s="33">
         <f t="shared" ref="D33:AA33" si="18">(2*(1-0.95))/(D25)</f>
-        <v>1.111111111111112E-2</v>
+        <v>1.2500000000000011E-2</v>
       </c>
       <c r="E33" s="33">
         <f t="shared" si="18"/>
@@ -8990,10 +8415,10 @@
       <c r="B34" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="C34" s="172"/>
+      <c r="C34" s="144"/>
       <c r="D34" s="34">
         <f t="shared" ref="D34:AA34" si="19">(D26-D20)/D27</f>
-        <v>2.1439767432000836</v>
+        <v>1.7338365504957904</v>
       </c>
       <c r="E34" s="34">
         <f t="shared" si="19"/>
@@ -9092,10 +8517,10 @@
       <c r="B35" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="C35" s="172"/>
+      <c r="C35" s="144"/>
       <c r="D35" s="34">
         <f t="shared" ref="D35:AA35" si="20">(D19-D26)/D27</f>
-        <v>0.9331028030509716</v>
+        <v>1.0462604009209311</v>
       </c>
       <c r="E35" s="34">
         <f t="shared" si="20"/>
@@ -9194,10 +8619,10 @@
       <c r="B36" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C36" s="172"/>
+      <c r="C36" s="144"/>
       <c r="D36" s="22">
         <f>VLOOKUP(D25,Distributions!$A$3:$C$40,(3))</f>
-        <v>2.11</v>
+        <v>2.032</v>
       </c>
       <c r="E36" s="22">
         <f>VLOOKUP(E25,Distributions!$A$3:$C$40,(3))</f>
@@ -9293,8 +8718,8 @@
       </c>
     </row>
     <row r="37" spans="2:27" ht="16.899999999999999" hidden="1" customHeight="1">
-      <c r="B37" s="176"/>
-      <c r="C37" s="177"/>
+      <c r="B37" s="148"/>
+      <c r="C37" s="149"/>
       <c r="D37" s="35"/>
       <c r="E37" s="35"/>
       <c r="F37" s="35"/>
@@ -9324,10 +8749,10 @@
       <c r="B38" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="C38" s="172"/>
+      <c r="C38" s="144"/>
       <c r="D38" s="22">
         <f>COUNTIF(SampleResults!B1:B32,"*")-1</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E38" s="22">
         <f>COUNTIF(SampleResults!C1:C32,"*")-1</f>
@@ -9426,10 +8851,10 @@
       <c r="B39" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="C39" s="172"/>
+      <c r="C39" s="144"/>
       <c r="D39" s="34">
         <f t="shared" ref="D39:AA39" si="21">SQRT(POWER(D27,2)+POWER(D27/SQRT(D25),2))</f>
-        <v>10.574909304108624</v>
+        <v>6.764334184846704</v>
       </c>
       <c r="E39" s="34">
         <f t="shared" si="21"/>
@@ -9528,10 +8953,10 @@
       <c r="B40" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="C40" s="172"/>
+      <c r="C40" s="144"/>
       <c r="D40" s="34">
         <f t="shared" ref="D40:AA40" si="22">IF(ISNUMBER(D7),D7,D28*D27)</f>
-        <v>29.053366562758992</v>
+        <v>19.119671338408814</v>
       </c>
       <c r="E40" s="34">
         <f t="shared" si="22"/>
@@ -9630,10 +9055,10 @@
       <c r="B41" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="C41" s="172"/>
+      <c r="C41" s="144"/>
       <c r="D41" s="34">
         <f t="shared" ref="D41:AA41" si="23">D39*2</f>
-        <v>21.149818608217249</v>
+        <v>13.528668369693408</v>
       </c>
       <c r="E41" s="34">
         <f t="shared" si="23"/>
@@ -9732,10 +9157,10 @@
       <c r="B42" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="C42" s="172"/>
+      <c r="C42" s="144"/>
       <c r="D42" s="38">
         <f t="shared" ref="D42:AA42" si="24">D26-D6</f>
-        <v>-9.5211111111111109</v>
+        <v>-6.8325000000000102</v>
       </c>
       <c r="E42" s="38">
         <f t="shared" si="24"/>
@@ -9834,10 +9259,10 @@
       <c r="B43" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="C43" s="172"/>
+      <c r="C43" s="144"/>
       <c r="D43" s="40">
         <f t="shared" ref="D43:AA43" si="25">IF(ISTEXT(D7),D13,IFERROR(D40/D16,IF(D7&gt;0,D7,D13)))</f>
-        <v>32.490545368467622</v>
+        <v>20.690418979250229</v>
       </c>
       <c r="E43" s="40">
         <f t="shared" si="25"/>
@@ -9936,10 +9361,10 @@
       <c r="B44" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="C44" s="178"/>
+      <c r="C44" s="150"/>
       <c r="D44" s="42">
         <f t="shared" ref="D44:AA44" si="26">D43*3</f>
-        <v>97.471636105402865</v>
+        <v>62.07125693775069</v>
       </c>
       <c r="E44" s="42">
         <f t="shared" si="26"/>
@@ -10038,10 +9463,10 @@
       <c r="B45" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="C45" s="178"/>
+      <c r="C45" s="150"/>
       <c r="D45" s="44" t="str">
         <f t="shared" ref="D45:AA45" si="27">FIXED(D44,((-1*INT(LOG10(D44)))-1)+D5,TRUE)</f>
-        <v>97</v>
+        <v>62</v>
       </c>
       <c r="E45" s="44" t="str">
         <f t="shared" si="27"/>
@@ -10140,7 +9565,7 @@
       <c r="B46" s="45" t="s">
         <v>37</v>
       </c>
-      <c r="C46" s="179"/>
+      <c r="C46" s="151"/>
       <c r="D46" s="46" t="str">
         <f t="shared" ref="D46:AA46" si="28">FIXED(D6,((-1*INT(LOG10(D6)))-1)+C5,TRUE)</f>
         <v>90</v>
@@ -10242,7 +9667,7 @@
       <c r="B47" s="45" t="s">
         <v>38</v>
       </c>
-      <c r="C47" s="178"/>
+      <c r="C47" s="150"/>
       <c r="D47" s="47"/>
       <c r="E47" s="47"/>
       <c r="F47" s="47"/>
@@ -10272,7 +9697,7 @@
       <c r="B48" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="C48" s="178"/>
+      <c r="C48" s="150"/>
       <c r="D48" s="48">
         <f t="shared" ref="D48:AA48" si="29">INT(LOG10(D46))</f>
         <v>1</v>
@@ -10374,7 +9799,7 @@
       <c r="B49" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="C49" s="178"/>
+      <c r="C49" s="150"/>
       <c r="D49" s="48">
         <f t="shared" ref="D49:AA49" si="30">INT(LOG10(D43))</f>
         <v>1</v>
@@ -10476,7 +9901,7 @@
       <c r="B50" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="C50" s="178"/>
+      <c r="C50" s="150"/>
       <c r="D50" s="42">
         <f t="shared" ref="D50:AA50" si="31">IF(D48=D49,1,D48-D49+1)</f>
         <v>1</v>
@@ -10578,10 +10003,10 @@
       <c r="B51" s="45" t="s">
         <v>42</v>
       </c>
-      <c r="C51" s="179"/>
+      <c r="C51" s="151"/>
       <c r="D51" s="44" t="str">
         <f t="shared" ref="D51:AA51" si="32">FIXED(D43,((-1*INT(LOG10(D43)))-D50)+D5,TRUE)</f>
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="E51" s="44" t="str">
         <f t="shared" si="32"/>
@@ -10678,7 +10103,7 @@
     </row>
     <row r="52" spans="2:27" ht="16.899999999999999" hidden="1" customHeight="1">
       <c r="B52" s="45"/>
-      <c r="C52" s="179"/>
+      <c r="C52" s="151"/>
       <c r="D52" s="47"/>
       <c r="E52" s="47"/>
       <c r="F52" s="47"/>
@@ -10704,110 +10129,115 @@
       <c r="Z52" s="47"/>
       <c r="AA52" s="47"/>
     </row>
-    <row r="53" spans="2:27" s="148" customFormat="1" ht="16.899999999999999" customHeight="1">
-      <c r="B53" s="114" t="s">
+    <row r="53" spans="2:27" s="139" customFormat="1" ht="16.899999999999999" customHeight="1">
+      <c r="B53" s="152" t="s">
         <v>106</v>
       </c>
-      <c r="C53" s="171"/>
-      <c r="D53" s="147" t="str">
+      <c r="C53" s="153"/>
+      <c r="D53" s="138" t="str">
         <f t="shared" ref="D53:AA53" si="33">IF(ISTEXT(D7),"MDL not a Number!",IFERROR(IF(D3="Blank","Blank: "&amp;D51&amp;" "&amp;IF(D7&gt;0,"^"&amp;D4,D4),IF(D7&gt;D6,"MDL &gt; Spike!",IF(D7&gt;0,D46&amp;" ± "&amp;D51&amp;" ^"&amp;D4,D46&amp;" ± "&amp;D51&amp;" "&amp;D4))),"Error!!"))</f>
-        <v>90 ± 32 µg/kg</v>
-      </c>
-      <c r="E53" s="147" t="str">
+        <v>90 ± 21 µg/kg</v>
+      </c>
+      <c r="E53" s="138" t="str">
         <f t="shared" si="33"/>
         <v>2.2 ± 0.6 µg/kg</v>
       </c>
-      <c r="F53" s="147" t="str">
+      <c r="F53" s="138" t="str">
         <f t="shared" si="33"/>
         <v>99 ± 12 µg/kg</v>
       </c>
-      <c r="G53" s="147" t="str">
+      <c r="G53" s="138" t="str">
         <f t="shared" si="33"/>
         <v>90 ± 42 µg/kg</v>
       </c>
-      <c r="H53" s="147" t="str">
+      <c r="H53" s="138" t="str">
         <f t="shared" si="33"/>
         <v>92 ± 383 µg/kg</v>
       </c>
-      <c r="I53" s="147" t="str">
+      <c r="I53" s="138" t="str">
         <f t="shared" si="33"/>
         <v>9.0 ± 1.8 µg/kg</v>
       </c>
-      <c r="J53" s="147" t="str">
+      <c r="J53" s="138" t="str">
         <f t="shared" si="33"/>
         <v>95 ± 19 µg/kg</v>
       </c>
-      <c r="K53" s="147" t="str">
+      <c r="K53" s="138" t="str">
         <f t="shared" si="33"/>
         <v>90 ± 37 µg/kg</v>
       </c>
-      <c r="L53" s="147" t="str">
+      <c r="L53" s="138" t="str">
         <f t="shared" si="33"/>
         <v>90 ± 19 µg/kg</v>
       </c>
-      <c r="M53" s="147" t="str">
+      <c r="M53" s="138" t="str">
         <f t="shared" si="33"/>
         <v>90 ± 1 ^µg/kg</v>
       </c>
-      <c r="N53" s="147" t="str">
+      <c r="N53" s="138" t="str">
         <f t="shared" si="33"/>
         <v>1.0 ± 0.2 µg/kg</v>
       </c>
-      <c r="O53" s="147" t="str">
+      <c r="O53" s="138" t="str">
         <f t="shared" si="33"/>
         <v>90 ± 25 µg/kg</v>
       </c>
-      <c r="P53" s="147" t="str">
+      <c r="P53" s="138" t="str">
         <f t="shared" si="33"/>
         <v>100 ± 20 µg/kg</v>
       </c>
-      <c r="Q53" s="147" t="str">
+      <c r="Q53" s="138" t="str">
         <f t="shared" si="33"/>
         <v>99 ± 21 µg/kg</v>
       </c>
-      <c r="R53" s="147" t="str">
+      <c r="R53" s="138" t="str">
         <f t="shared" si="33"/>
         <v>90 ± 29 µg/kg</v>
       </c>
-      <c r="S53" s="147" t="str">
+      <c r="S53" s="138" t="str">
         <f t="shared" si="33"/>
         <v>93 ± 27 µg/kg</v>
       </c>
-      <c r="T53" s="147" t="str">
+      <c r="T53" s="138" t="str">
         <f t="shared" si="33"/>
         <v>110 ± 20 µg/kg</v>
       </c>
-      <c r="U53" s="147" t="str">
+      <c r="U53" s="138" t="str">
         <f t="shared" si="33"/>
         <v>90 ± 20 µg/kg</v>
       </c>
-      <c r="V53" s="147" t="str">
+      <c r="V53" s="138" t="str">
         <f t="shared" si="33"/>
         <v>0.0010 ± 0.0003 µg/kg</v>
       </c>
-      <c r="W53" s="147" t="str">
+      <c r="W53" s="138" t="str">
         <f t="shared" si="33"/>
         <v>110 ± 30 µg/kg</v>
       </c>
-      <c r="X53" s="147" t="str">
+      <c r="X53" s="138" t="str">
         <f t="shared" si="33"/>
         <v>1.2 ± 0.4 µg/kg</v>
       </c>
-      <c r="Y53" s="147" t="str">
+      <c r="Y53" s="138" t="str">
         <f t="shared" si="33"/>
         <v>0.12 ± 0.04 µg/kg</v>
       </c>
-      <c r="Z53" s="147" t="str">
+      <c r="Z53" s="138" t="str">
         <f t="shared" si="33"/>
         <v>0.012 ± 0.004 µg/kg</v>
       </c>
-      <c r="AA53" s="147" t="str">
+      <c r="AA53" s="138" t="str">
         <f t="shared" si="33"/>
         <v>1200 ± 200 µg/kg</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
     <mergeCell ref="B53:C53"/>
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="B6:C6"/>
@@ -10822,11 +10252,6 @@
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
   </mergeCells>
   <conditionalFormatting sqref="C5">
     <cfRule type="cellIs" dxfId="36" priority="6" stopIfTrue="1" operator="notEqual">
@@ -10999,94 +10424,94 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFD32"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="Y11" sqref="Y11"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1"/>
   <cols>
-    <col min="1" max="1" width="14.1875" style="130" customWidth="1"/>
-    <col min="2" max="2" width="10.375" style="131" customWidth="1"/>
-    <col min="3" max="24" width="10.5" style="128" customWidth="1"/>
-    <col min="25" max="25" width="10.5" style="137" customWidth="1"/>
-    <col min="26" max="16383" width="8.875" style="128" hidden="1"/>
-    <col min="16384" max="16384" width="6.25E-2" style="138" customWidth="1"/>
+    <col min="1" max="1" width="14.1875" style="123" customWidth="1"/>
+    <col min="2" max="2" width="10.375" style="124" customWidth="1"/>
+    <col min="3" max="24" width="10.5" style="121" customWidth="1"/>
+    <col min="25" max="25" width="10.5" style="130" customWidth="1"/>
+    <col min="26" max="16383" width="8.875" style="121" hidden="1"/>
+    <col min="16384" max="16384" width="6.25E-2" style="131" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="16.600000000000001" customHeight="1">
-      <c r="A1" s="124" t="s">
+      <c r="A1" s="117" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="125" t="s">
+      <c r="B1" s="118" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="126" t="s">
+      <c r="C1" s="119" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="126" t="s">
+      <c r="D1" s="119" t="s">
         <v>46</v>
       </c>
-      <c r="E1" s="126" t="s">
+      <c r="E1" s="119" t="s">
         <v>47</v>
       </c>
-      <c r="F1" s="126" t="s">
+      <c r="F1" s="119" t="s">
         <v>48</v>
       </c>
-      <c r="G1" s="126" t="s">
+      <c r="G1" s="119" t="s">
         <v>49</v>
       </c>
-      <c r="H1" s="126" t="s">
+      <c r="H1" s="119" t="s">
         <v>50</v>
       </c>
-      <c r="I1" s="126" t="s">
+      <c r="I1" s="119" t="s">
         <v>51</v>
       </c>
-      <c r="J1" s="126" t="s">
+      <c r="J1" s="119" t="s">
         <v>52</v>
       </c>
-      <c r="K1" s="127" t="s">
+      <c r="K1" s="120" t="s">
         <v>53</v>
       </c>
-      <c r="L1" s="127" t="s">
+      <c r="L1" s="120" t="s">
         <v>54</v>
       </c>
-      <c r="M1" s="127" t="s">
+      <c r="M1" s="120" t="s">
         <v>55</v>
       </c>
-      <c r="N1" s="127" t="s">
+      <c r="N1" s="120" t="s">
         <v>56</v>
       </c>
-      <c r="O1" s="127" t="s">
+      <c r="O1" s="120" t="s">
         <v>57</v>
       </c>
-      <c r="P1" s="127" t="s">
+      <c r="P1" s="120" t="s">
         <v>58</v>
       </c>
-      <c r="Q1" s="127" t="s">
+      <c r="Q1" s="120" t="s">
         <v>59</v>
       </c>
-      <c r="R1" s="127" t="s">
+      <c r="R1" s="120" t="s">
         <v>60</v>
       </c>
-      <c r="S1" s="127" t="s">
+      <c r="S1" s="120" t="s">
         <v>61</v>
       </c>
-      <c r="T1" s="127" t="s">
+      <c r="T1" s="120" t="s">
         <v>62</v>
       </c>
-      <c r="U1" s="127" t="s">
+      <c r="U1" s="120" t="s">
         <v>63</v>
       </c>
-      <c r="V1" s="127" t="s">
+      <c r="V1" s="120" t="s">
         <v>64</v>
       </c>
-      <c r="W1" s="127" t="s">
+      <c r="W1" s="120" t="s">
         <v>65</v>
       </c>
-      <c r="X1" s="127" t="s">
+      <c r="X1" s="120" t="s">
         <v>66</v>
       </c>
-      <c r="Y1" s="134" t="s">
+      <c r="Y1" s="127" t="s">
         <v>67</v>
       </c>
     </row>
@@ -11094,1320 +10519,1320 @@
       <c r="A2" s="110" t="s">
         <v>68</v>
       </c>
-      <c r="B2" s="120">
+      <c r="B2" s="113">
         <v>86.38</v>
       </c>
-      <c r="C2" s="120">
+      <c r="C2" s="113">
         <v>1.59</v>
       </c>
-      <c r="D2" s="120">
+      <c r="D2" s="113">
         <v>94.21</v>
       </c>
-      <c r="E2" s="120">
+      <c r="E2" s="113">
         <v>94.21</v>
       </c>
-      <c r="F2" s="120">
+      <c r="F2" s="113">
         <v>86.38</v>
       </c>
-      <c r="G2" s="120">
+      <c r="G2" s="113">
         <v>9.0299999999999994</v>
       </c>
-      <c r="H2" s="120">
+      <c r="H2" s="113">
         <v>96</v>
       </c>
-      <c r="I2" s="120">
+      <c r="I2" s="113">
         <v>86.38</v>
       </c>
-      <c r="J2" s="120">
+      <c r="J2" s="113">
         <v>90</v>
       </c>
-      <c r="K2" s="120">
+      <c r="K2" s="113">
         <v>96.1</v>
       </c>
-      <c r="L2" s="120">
+      <c r="L2" s="113">
         <v>0.85099999999999998</v>
       </c>
-      <c r="M2" s="120">
+      <c r="M2" s="113">
         <v>90</v>
       </c>
-      <c r="N2" s="120">
+      <c r="N2" s="113">
         <v>90</v>
       </c>
-      <c r="O2" s="120">
+      <c r="O2" s="113">
         <v>86.38</v>
       </c>
-      <c r="P2" s="120">
+      <c r="P2" s="113">
         <v>90</v>
       </c>
-      <c r="Q2" s="120">
+      <c r="Q2" s="113">
         <v>84</v>
       </c>
-      <c r="R2" s="120">
+      <c r="R2" s="113">
         <v>86.38</v>
       </c>
-      <c r="S2" s="120">
+      <c r="S2" s="113">
         <v>96</v>
       </c>
-      <c r="T2" s="120">
+      <c r="T2" s="113">
         <v>1.0300000000000001E-3</v>
       </c>
-      <c r="U2" s="120">
+      <c r="U2" s="113">
         <v>86.38</v>
       </c>
-      <c r="V2" s="120">
+      <c r="V2" s="113">
         <v>1.03</v>
       </c>
-      <c r="W2" s="120">
+      <c r="W2" s="113">
         <v>0.10299999999999999</v>
       </c>
-      <c r="X2" s="120">
+      <c r="X2" s="113">
         <v>1.03E-2</v>
       </c>
-      <c r="Y2" s="135">
+      <c r="Y2" s="128">
         <v>962</v>
       </c>
-      <c r="Z2" s="132"/>
+      <c r="Z2" s="125"/>
     </row>
     <row r="3" spans="1:26" ht="16.600000000000001" customHeight="1">
       <c r="A3" s="111" t="s">
         <v>69</v>
       </c>
-      <c r="B3" s="121">
+      <c r="B3" s="114">
         <v>87.79</v>
       </c>
-      <c r="C3" s="120">
+      <c r="C3" s="113">
         <v>1.66</v>
       </c>
-      <c r="D3" s="120">
+      <c r="D3" s="113">
         <v>91.3</v>
       </c>
-      <c r="E3" s="120">
+      <c r="E3" s="113">
         <v>88.46</v>
       </c>
-      <c r="F3" s="120">
+      <c r="F3" s="113">
         <v>87.79</v>
       </c>
-      <c r="G3" s="120">
+      <c r="G3" s="113">
         <v>9.11</v>
       </c>
-      <c r="H3" s="120">
+      <c r="H3" s="113">
         <v>97</v>
       </c>
-      <c r="I3" s="120">
+      <c r="I3" s="113">
         <v>87.79</v>
       </c>
-      <c r="J3" s="120">
+      <c r="J3" s="113">
         <v>84</v>
       </c>
-      <c r="K3" s="120">
+      <c r="K3" s="113">
         <v>90.1</v>
       </c>
-      <c r="L3" s="120">
+      <c r="L3" s="113">
         <v>0.88200000000000001</v>
       </c>
-      <c r="M3" s="120">
+      <c r="M3" s="113">
         <v>91</v>
       </c>
-      <c r="N3" s="120">
+      <c r="N3" s="113">
         <v>104</v>
       </c>
-      <c r="O3" s="120">
+      <c r="O3" s="113">
         <v>87.79</v>
       </c>
-      <c r="P3" s="120">
+      <c r="P3" s="113">
         <v>91</v>
       </c>
-      <c r="Q3" s="120">
+      <c r="Q3" s="113">
         <v>97</v>
       </c>
-      <c r="R3" s="120">
+      <c r="R3" s="113">
         <v>87.79</v>
       </c>
-      <c r="S3" s="120">
+      <c r="S3" s="113">
         <v>97</v>
       </c>
-      <c r="T3" s="120">
+      <c r="T3" s="113">
         <v>1.2199999999999999E-3</v>
       </c>
-      <c r="U3" s="120">
+      <c r="U3" s="113">
         <v>87.79</v>
       </c>
-      <c r="V3" s="120">
+      <c r="V3" s="113">
         <v>1.2</v>
       </c>
-      <c r="W3" s="120">
+      <c r="W3" s="113">
         <v>0.12</v>
       </c>
-      <c r="X3" s="120">
+      <c r="X3" s="113">
         <v>1.2E-2</v>
       </c>
-      <c r="Y3" s="135">
+      <c r="Y3" s="128">
         <v>973</v>
       </c>
-      <c r="Z3" s="132"/>
+      <c r="Z3" s="125"/>
     </row>
     <row r="4" spans="1:26" ht="16.600000000000001" customHeight="1">
       <c r="A4" s="111" t="s">
         <v>70</v>
       </c>
-      <c r="B4" s="120">
+      <c r="B4" s="113">
         <v>77.94</v>
       </c>
-      <c r="C4" s="120">
+      <c r="C4" s="113">
         <v>1.42</v>
       </c>
-      <c r="D4" s="120">
+      <c r="D4" s="113">
         <v>91.88</v>
       </c>
-      <c r="E4" s="120">
+      <c r="E4" s="113">
         <v>98.27</v>
       </c>
-      <c r="F4" s="120">
+      <c r="F4" s="113">
         <v>77.94</v>
       </c>
-      <c r="G4" s="120">
+      <c r="G4" s="113">
         <v>9.24</v>
       </c>
-      <c r="H4" s="120">
+      <c r="H4" s="113">
         <v>98</v>
       </c>
-      <c r="I4" s="120">
+      <c r="I4" s="113">
         <v>77.94</v>
       </c>
-      <c r="J4" s="120">
+      <c r="J4" s="113">
         <v>101</v>
       </c>
-      <c r="K4" s="120">
+      <c r="K4" s="113">
         <v>95.2</v>
       </c>
-      <c r="L4" s="120">
+      <c r="L4" s="113">
         <v>0.77900000000000003</v>
       </c>
-      <c r="M4" s="120">
+      <c r="M4" s="113">
         <v>92</v>
       </c>
-      <c r="N4" s="120">
+      <c r="N4" s="113">
         <v>93</v>
       </c>
-      <c r="O4" s="120">
+      <c r="O4" s="113">
         <v>77.94</v>
       </c>
-      <c r="P4" s="120">
+      <c r="P4" s="113">
         <v>92</v>
       </c>
-      <c r="Q4" s="120">
+      <c r="Q4" s="113">
         <v>98</v>
       </c>
-      <c r="R4" s="120">
+      <c r="R4" s="113">
         <v>77.94</v>
       </c>
-      <c r="S4" s="120">
+      <c r="S4" s="113">
         <v>88</v>
       </c>
-      <c r="T4" s="120">
+      <c r="T4" s="113">
         <v>1.25E-3</v>
       </c>
-      <c r="U4" s="120">
+      <c r="U4" s="113">
         <v>77.94</v>
       </c>
-      <c r="V4" s="120">
+      <c r="V4" s="113">
         <v>1.25</v>
       </c>
-      <c r="W4" s="120">
+      <c r="W4" s="113">
         <v>0.125</v>
       </c>
-      <c r="X4" s="120">
+      <c r="X4" s="113">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="Y4" s="135">
+      <c r="Y4" s="128">
         <v>981</v>
       </c>
-      <c r="Z4" s="132"/>
+      <c r="Z4" s="125"/>
     </row>
     <row r="5" spans="1:26" ht="16.600000000000001" customHeight="1">
       <c r="A5" s="111" t="s">
         <v>71</v>
       </c>
-      <c r="B5" s="121">
+      <c r="B5" s="114">
         <v>72.11</v>
       </c>
-      <c r="C5" s="120">
+      <c r="C5" s="113">
         <v>1.59</v>
       </c>
-      <c r="D5" s="120">
+      <c r="D5" s="113">
         <v>95.31</v>
       </c>
-      <c r="E5" s="120">
+      <c r="E5" s="113">
         <v>99.41</v>
       </c>
-      <c r="F5" s="120">
+      <c r="F5" s="113">
         <v>72.11</v>
       </c>
-      <c r="G5" s="120">
+      <c r="G5" s="113">
         <v>9.35</v>
       </c>
-      <c r="H5" s="120">
+      <c r="H5" s="113">
         <v>83</v>
       </c>
-      <c r="I5" s="120">
+      <c r="I5" s="113">
         <v>72.11</v>
       </c>
-      <c r="J5" s="120">
+      <c r="J5" s="113">
         <v>93</v>
       </c>
-      <c r="K5" s="120">
+      <c r="K5" s="113">
         <v>91.3</v>
       </c>
-      <c r="L5" s="120">
+      <c r="L5" s="113">
         <v>0.72099999999999997</v>
       </c>
-      <c r="M5" s="120">
+      <c r="M5" s="113">
         <v>93</v>
       </c>
-      <c r="N5" s="120">
+      <c r="N5" s="113">
         <v>89</v>
       </c>
-      <c r="O5" s="120">
+      <c r="O5" s="113">
         <v>72.11</v>
       </c>
-      <c r="P5" s="120">
+      <c r="P5" s="113">
         <v>93</v>
       </c>
-      <c r="Q5" s="120">
+      <c r="Q5" s="113">
         <v>99</v>
       </c>
-      <c r="R5" s="120">
+      <c r="R5" s="113">
         <v>72.11</v>
       </c>
-      <c r="S5" s="120">
+      <c r="S5" s="113">
         <v>99</v>
       </c>
-      <c r="T5" s="120">
+      <c r="T5" s="113">
         <v>1.33E-3</v>
       </c>
-      <c r="U5" s="120">
+      <c r="U5" s="113">
         <v>72.11</v>
       </c>
-      <c r="V5" s="120">
+      <c r="V5" s="113">
         <v>1.33</v>
       </c>
-      <c r="W5" s="120">
+      <c r="W5" s="113">
         <v>0.13300000000000001</v>
       </c>
-      <c r="X5" s="120">
+      <c r="X5" s="113">
         <v>1.3299999999999999E-2</v>
       </c>
-      <c r="Y5" s="135">
+      <c r="Y5" s="128">
         <v>989</v>
       </c>
-      <c r="Z5" s="132"/>
+      <c r="Z5" s="125"/>
     </row>
     <row r="6" spans="1:26" ht="16.600000000000001" customHeight="1">
       <c r="A6" s="111" t="s">
         <v>72</v>
       </c>
-      <c r="B6" s="121">
+      <c r="B6" s="114">
         <v>78.56</v>
       </c>
-      <c r="C6" s="120">
+      <c r="C6" s="113">
         <v>1.66</v>
       </c>
-      <c r="D6" s="120">
+      <c r="D6" s="113">
         <v>94.69</v>
       </c>
-      <c r="E6" s="120">
+      <c r="E6" s="113">
         <v>100.24</v>
       </c>
-      <c r="F6" s="120">
+      <c r="F6" s="113">
         <v>78.56</v>
       </c>
-      <c r="G6" s="120">
+      <c r="G6" s="113">
         <v>9.06</v>
       </c>
-      <c r="H6" s="120">
+      <c r="H6" s="113">
         <v>100</v>
       </c>
-      <c r="I6" s="120">
+      <c r="I6" s="113">
         <v>78.56</v>
       </c>
-      <c r="J6" s="120">
+      <c r="J6" s="113">
         <v>85</v>
       </c>
-      <c r="K6" s="120">
+      <c r="K6" s="113">
         <v>100.2</v>
       </c>
-      <c r="L6" s="120">
+      <c r="L6" s="113">
         <v>0.78600000000000003</v>
       </c>
-      <c r="M6" s="120">
+      <c r="M6" s="113">
         <v>94</v>
       </c>
-      <c r="N6" s="120">
+      <c r="N6" s="113">
         <v>100</v>
       </c>
-      <c r="O6" s="120">
+      <c r="O6" s="113">
         <v>78.56</v>
       </c>
-      <c r="P6" s="120">
+      <c r="P6" s="113">
         <v>94</v>
       </c>
-      <c r="Q6" s="120">
+      <c r="Q6" s="113">
         <v>100</v>
       </c>
-      <c r="R6" s="120">
+      <c r="R6" s="113">
         <v>78.56</v>
       </c>
-      <c r="S6" s="120">
+      <c r="S6" s="113">
         <v>100</v>
       </c>
-      <c r="T6" s="120">
+      <c r="T6" s="113">
         <v>1.4599999999999999E-3</v>
       </c>
-      <c r="U6" s="120">
+      <c r="U6" s="113">
         <v>78.56</v>
       </c>
-      <c r="V6" s="120">
+      <c r="V6" s="113">
         <v>1.46</v>
       </c>
-      <c r="W6" s="120">
+      <c r="W6" s="113">
         <v>0.14599999999999999</v>
       </c>
-      <c r="X6" s="120">
+      <c r="X6" s="113">
         <v>1.46E-2</v>
       </c>
-      <c r="Y6" s="135">
+      <c r="Y6" s="128">
         <v>951</v>
       </c>
-      <c r="Z6" s="132"/>
+      <c r="Z6" s="125"/>
     </row>
     <row r="7" spans="1:26" ht="16.600000000000001" customHeight="1">
       <c r="A7" s="111" t="s">
         <v>73</v>
       </c>
-      <c r="B7" s="121">
+      <c r="B7" s="114">
         <v>89.84</v>
       </c>
-      <c r="C7" s="120">
+      <c r="C7" s="113">
         <v>1.36</v>
       </c>
-      <c r="D7" s="120">
+      <c r="D7" s="113">
         <v>85.37</v>
       </c>
-      <c r="E7" s="120">
+      <c r="E7" s="113">
         <v>100.91</v>
       </c>
-      <c r="F7" s="120">
+      <c r="F7" s="113">
         <v>89.84</v>
       </c>
-      <c r="G7" s="120">
+      <c r="G7" s="113">
         <v>9.4700000000000006</v>
       </c>
-      <c r="H7" s="120">
+      <c r="H7" s="113">
         <v>101</v>
       </c>
-      <c r="I7" s="120">
+      <c r="I7" s="113">
         <v>89.84</v>
       </c>
-      <c r="J7" s="120">
+      <c r="J7" s="113">
         <v>95</v>
       </c>
-      <c r="K7" s="120">
+      <c r="K7" s="113">
         <v>111.3</v>
       </c>
-      <c r="L7" s="120">
+      <c r="L7" s="113">
         <v>0.89800000000000002</v>
       </c>
-      <c r="M7" s="120">
+      <c r="M7" s="113">
         <v>95</v>
       </c>
-      <c r="N7" s="120">
+      <c r="N7" s="113">
         <v>91</v>
       </c>
-      <c r="O7" s="120">
+      <c r="O7" s="113">
         <v>89.84</v>
       </c>
-      <c r="P7" s="120">
+      <c r="P7" s="113">
         <v>95</v>
       </c>
-      <c r="Q7" s="120">
+      <c r="Q7" s="113">
         <v>101</v>
       </c>
-      <c r="R7" s="120">
+      <c r="R7" s="113">
         <v>89.84</v>
       </c>
-      <c r="S7" s="120">
+      <c r="S7" s="113">
         <v>101</v>
       </c>
-      <c r="T7" s="120">
+      <c r="T7" s="113">
         <v>1.3699999999999999E-3</v>
       </c>
-      <c r="U7" s="120">
+      <c r="U7" s="113">
         <v>89.84</v>
       </c>
-      <c r="V7" s="120">
+      <c r="V7" s="113">
         <v>1.371</v>
       </c>
-      <c r="W7" s="120">
+      <c r="W7" s="113">
         <v>0.1371</v>
       </c>
-      <c r="X7" s="120">
+      <c r="X7" s="113">
         <v>1.37E-2</v>
       </c>
-      <c r="Y7" s="135">
+      <c r="Y7" s="128">
         <v>1005</v>
       </c>
-      <c r="Z7" s="132"/>
+      <c r="Z7" s="125"/>
     </row>
     <row r="8" spans="1:26" ht="16.600000000000001" customHeight="1">
       <c r="A8" s="111" t="s">
         <v>74</v>
       </c>
-      <c r="B8" s="121">
+      <c r="B8" s="114">
         <v>89.3</v>
       </c>
-      <c r="C8" s="120">
+      <c r="C8" s="113">
         <v>1.69</v>
       </c>
-      <c r="D8" s="120">
+      <c r="D8" s="113">
         <v>99.21</v>
       </c>
-      <c r="E8" s="120">
+      <c r="E8" s="113">
         <v>81.31</v>
       </c>
-      <c r="F8" s="120">
+      <c r="F8" s="113">
         <v>89.3</v>
       </c>
-      <c r="G8" s="120">
+      <c r="G8" s="113">
         <v>9.91</v>
       </c>
-      <c r="H8" s="120">
+      <c r="H8" s="113">
         <v>102</v>
       </c>
-      <c r="I8" s="120">
+      <c r="I8" s="113">
         <v>89.3</v>
       </c>
-      <c r="J8" s="120">
+      <c r="J8" s="113">
         <v>99</v>
       </c>
-      <c r="K8" s="120">
+      <c r="K8" s="113">
         <v>102.4</v>
       </c>
-      <c r="L8" s="120">
+      <c r="L8" s="113">
         <v>0.89300000000000002</v>
       </c>
-      <c r="M8" s="120">
+      <c r="M8" s="113">
         <v>99</v>
       </c>
-      <c r="N8" s="120">
+      <c r="N8" s="113">
         <v>102</v>
       </c>
-      <c r="O8" s="120">
+      <c r="O8" s="113">
         <v>89.3</v>
       </c>
-      <c r="P8" s="120">
+      <c r="P8" s="113">
         <v>99</v>
       </c>
-      <c r="Q8" s="120">
+      <c r="Q8" s="113">
         <v>102</v>
       </c>
-      <c r="R8" s="120">
+      <c r="R8" s="113">
         <v>89.3</v>
       </c>
-      <c r="S8" s="120">
+      <c r="S8" s="113">
         <v>102</v>
       </c>
-      <c r="T8" s="120">
+      <c r="T8" s="113">
         <v>1.14E-3</v>
       </c>
-      <c r="U8" s="120">
+      <c r="U8" s="113">
         <v>89.3</v>
       </c>
-      <c r="V8" s="120">
+      <c r="V8" s="113">
         <v>1.1379999999999999</v>
       </c>
-      <c r="W8" s="120">
+      <c r="W8" s="113">
         <v>0.1138</v>
       </c>
-      <c r="X8" s="120">
+      <c r="X8" s="113">
         <v>1.14E-2</v>
       </c>
-      <c r="Y8" s="135">
+      <c r="Y8" s="128">
         <v>1024</v>
       </c>
-      <c r="Z8" s="132"/>
+      <c r="Z8" s="125"/>
     </row>
     <row r="9" spans="1:26" ht="16.600000000000001" customHeight="1">
       <c r="A9" s="111" t="s">
         <v>75</v>
       </c>
-      <c r="B9" s="121">
+      <c r="B9" s="114">
         <v>83.42</v>
       </c>
-      <c r="C9" s="120">
+      <c r="C9" s="113">
         <v>1.82</v>
       </c>
-      <c r="D9" s="120">
+      <c r="D9" s="113">
         <v>96.33</v>
       </c>
-      <c r="E9" s="120">
+      <c r="E9" s="113">
         <v>107.18</v>
       </c>
-      <c r="F9" s="120">
+      <c r="F9" s="113">
         <v>83.42</v>
       </c>
-      <c r="G9" s="120">
+      <c r="G9" s="113">
         <v>8.07</v>
       </c>
-      <c r="H9" s="120">
+      <c r="H9" s="113">
         <v>90</v>
       </c>
-      <c r="I9" s="120">
+      <c r="I9" s="113">
         <v>83.42</v>
       </c>
-      <c r="J9" s="120">
+      <c r="J9" s="113">
         <v>103</v>
       </c>
-      <c r="K9" s="120">
+      <c r="K9" s="113">
         <v>101.6</v>
       </c>
-      <c r="L9" s="120">
+      <c r="L9" s="113">
         <v>0.83299999999999996</v>
       </c>
-      <c r="M9" s="120">
+      <c r="M9" s="113">
         <v>117</v>
       </c>
-      <c r="N9" s="120">
+      <c r="N9" s="113">
         <v>103</v>
       </c>
-      <c r="O9" s="120">
+      <c r="O9" s="113">
         <v>83.42</v>
       </c>
-      <c r="P9" s="120">
+      <c r="P9" s="113">
         <v>121</v>
       </c>
-      <c r="Q9" s="120">
+      <c r="Q9" s="113">
         <v>110</v>
       </c>
-      <c r="R9" s="120">
+      <c r="R9" s="113">
         <v>83.42</v>
       </c>
-      <c r="S9" s="120">
+      <c r="S9" s="113">
         <v>106</v>
       </c>
-      <c r="T9" s="120">
+      <c r="T9" s="113">
         <v>1.1349999999999999E-3</v>
       </c>
-      <c r="U9" s="120">
+      <c r="U9" s="113">
         <v>83.42</v>
       </c>
-      <c r="V9" s="120">
+      <c r="V9" s="113">
         <v>1.135</v>
       </c>
-      <c r="W9" s="120">
+      <c r="W9" s="113">
         <v>0.1135</v>
       </c>
-      <c r="X9" s="120">
+      <c r="X9" s="113">
         <v>1.1299999999999999E-2</v>
       </c>
-      <c r="Y9" s="135">
+      <c r="Y9" s="128">
         <v>1056</v>
       </c>
-      <c r="Z9" s="132"/>
+      <c r="Z9" s="125"/>
     </row>
     <row r="10" spans="1:26" ht="14.65" customHeight="1">
       <c r="A10" s="111" t="s">
         <v>76</v>
       </c>
-      <c r="B10" s="120">
-        <v>58.97</v>
-      </c>
-      <c r="C10" s="120">
+      <c r="B10" s="113" t="s">
+        <v>107</v>
+      </c>
+      <c r="C10" s="113">
         <v>1.67</v>
       </c>
-      <c r="D10" s="120">
+      <c r="D10" s="113">
         <v>92.02</v>
       </c>
-      <c r="E10" s="120">
+      <c r="E10" s="113">
         <v>140.1</v>
       </c>
-      <c r="F10" s="120">
+      <c r="F10" s="113">
         <v>771</v>
       </c>
-      <c r="G10" s="120">
+      <c r="G10" s="113">
         <v>10.4</v>
       </c>
-      <c r="H10" s="120">
+      <c r="H10" s="113">
         <v>106</v>
       </c>
-      <c r="I10" s="120">
+      <c r="I10" s="113">
         <v>53.77</v>
       </c>
-      <c r="J10" s="120">
+      <c r="J10" s="113">
         <v>88</v>
       </c>
-      <c r="K10" s="120">
+      <c r="K10" s="113">
         <v>103.7</v>
       </c>
-      <c r="L10" s="120">
+      <c r="L10" s="113">
         <v>0.88400000000000001</v>
       </c>
-      <c r="M10" s="120">
+      <c r="M10" s="113">
         <v>111</v>
       </c>
-      <c r="N10" s="120">
+      <c r="N10" s="113">
         <v>106</v>
       </c>
-      <c r="O10" s="120">
+      <c r="O10" s="113">
         <v>81</v>
       </c>
-      <c r="P10" s="120">
+      <c r="P10" s="113">
         <v>114</v>
       </c>
-      <c r="Q10" s="120">
+      <c r="Q10" s="113">
         <v>122</v>
       </c>
-      <c r="R10" s="120">
+      <c r="R10" s="113">
         <v>82</v>
       </c>
-      <c r="S10" s="120">
+      <c r="S10" s="113">
         <v>117</v>
       </c>
-      <c r="T10" s="120">
+      <c r="T10" s="113">
         <v>1.17E-3</v>
       </c>
-      <c r="U10" s="120">
+      <c r="U10" s="113">
         <v>68.430000000000007</v>
       </c>
-      <c r="V10" s="120">
+      <c r="V10" s="113">
         <v>1.1739999999999999</v>
       </c>
-      <c r="W10" s="120">
+      <c r="W10" s="113">
         <v>0.1174</v>
       </c>
-      <c r="X10" s="120">
+      <c r="X10" s="113">
         <v>1.17E-2</v>
       </c>
-      <c r="Y10" s="135">
+      <c r="Y10" s="128">
         <v>1100</v>
       </c>
-      <c r="Z10" s="132"/>
+      <c r="Z10" s="125"/>
     </row>
     <row r="11" spans="1:26" ht="16.600000000000001" customHeight="1">
       <c r="A11" s="111"/>
-      <c r="B11" s="120"/>
-      <c r="C11" s="120"/>
-      <c r="D11" s="120"/>
-      <c r="E11" s="120"/>
-      <c r="F11" s="120"/>
-      <c r="G11" s="120"/>
-      <c r="H11" s="120"/>
-      <c r="I11" s="120"/>
-      <c r="J11" s="120"/>
-      <c r="K11" s="120"/>
-      <c r="L11" s="120"/>
-      <c r="M11" s="120"/>
-      <c r="N11" s="120"/>
-      <c r="O11" s="120"/>
-      <c r="P11" s="120"/>
-      <c r="Q11" s="120"/>
-      <c r="R11" s="120"/>
-      <c r="S11" s="120"/>
-      <c r="T11" s="120"/>
-      <c r="U11" s="120"/>
-      <c r="V11" s="120"/>
-      <c r="W11" s="120"/>
-      <c r="X11" s="120"/>
-      <c r="Y11" s="135"/>
-      <c r="Z11" s="132"/>
+      <c r="B11" s="113"/>
+      <c r="C11" s="113"/>
+      <c r="D11" s="113"/>
+      <c r="E11" s="113"/>
+      <c r="F11" s="113"/>
+      <c r="G11" s="113"/>
+      <c r="H11" s="113"/>
+      <c r="I11" s="113"/>
+      <c r="J11" s="113"/>
+      <c r="K11" s="113"/>
+      <c r="L11" s="113"/>
+      <c r="M11" s="113"/>
+      <c r="N11" s="113"/>
+      <c r="O11" s="113"/>
+      <c r="P11" s="113"/>
+      <c r="Q11" s="113"/>
+      <c r="R11" s="113"/>
+      <c r="S11" s="113"/>
+      <c r="T11" s="113"/>
+      <c r="U11" s="113"/>
+      <c r="V11" s="113"/>
+      <c r="W11" s="113"/>
+      <c r="X11" s="113"/>
+      <c r="Y11" s="128"/>
+      <c r="Z11" s="125"/>
     </row>
     <row r="12" spans="1:26" ht="16.600000000000001" customHeight="1">
       <c r="A12" s="111"/>
-      <c r="B12" s="121"/>
-      <c r="C12" s="120"/>
-      <c r="D12" s="120"/>
-      <c r="E12" s="120"/>
-      <c r="F12" s="120"/>
-      <c r="G12" s="120"/>
-      <c r="H12" s="120"/>
-      <c r="I12" s="120"/>
-      <c r="J12" s="120"/>
-      <c r="K12" s="120"/>
-      <c r="L12" s="120"/>
-      <c r="M12" s="120"/>
-      <c r="N12" s="120"/>
-      <c r="O12" s="120"/>
-      <c r="P12" s="120"/>
-      <c r="Q12" s="120"/>
-      <c r="R12" s="120"/>
-      <c r="S12" s="120"/>
-      <c r="T12" s="120"/>
-      <c r="U12" s="120"/>
-      <c r="V12" s="120"/>
-      <c r="W12" s="120"/>
-      <c r="X12" s="120"/>
-      <c r="Y12" s="135"/>
-      <c r="Z12" s="132"/>
+      <c r="B12" s="114"/>
+      <c r="C12" s="113"/>
+      <c r="D12" s="113"/>
+      <c r="E12" s="113"/>
+      <c r="F12" s="113"/>
+      <c r="G12" s="113"/>
+      <c r="H12" s="113"/>
+      <c r="I12" s="113"/>
+      <c r="J12" s="113"/>
+      <c r="K12" s="113"/>
+      <c r="L12" s="113"/>
+      <c r="M12" s="113"/>
+      <c r="N12" s="113"/>
+      <c r="O12" s="113"/>
+      <c r="P12" s="113"/>
+      <c r="Q12" s="113"/>
+      <c r="R12" s="113"/>
+      <c r="S12" s="113"/>
+      <c r="T12" s="113"/>
+      <c r="U12" s="113"/>
+      <c r="V12" s="113"/>
+      <c r="W12" s="113"/>
+      <c r="X12" s="113"/>
+      <c r="Y12" s="128"/>
+      <c r="Z12" s="125"/>
     </row>
     <row r="13" spans="1:26" ht="16.600000000000001" customHeight="1">
       <c r="A13" s="111"/>
-      <c r="B13" s="121"/>
-      <c r="C13" s="120"/>
-      <c r="D13" s="120"/>
-      <c r="E13" s="120"/>
-      <c r="F13" s="120"/>
-      <c r="G13" s="120"/>
-      <c r="H13" s="120"/>
-      <c r="I13" s="120"/>
-      <c r="J13" s="120"/>
-      <c r="K13" s="120"/>
-      <c r="L13" s="120"/>
-      <c r="M13" s="120"/>
-      <c r="N13" s="120"/>
-      <c r="O13" s="120"/>
-      <c r="P13" s="120"/>
-      <c r="Q13" s="120"/>
-      <c r="R13" s="120"/>
-      <c r="S13" s="120"/>
-      <c r="T13" s="120"/>
-      <c r="U13" s="120"/>
-      <c r="V13" s="120"/>
-      <c r="W13" s="120"/>
-      <c r="X13" s="120"/>
-      <c r="Y13" s="135"/>
-      <c r="Z13" s="132"/>
+      <c r="B13" s="114"/>
+      <c r="C13" s="113"/>
+      <c r="D13" s="113"/>
+      <c r="E13" s="113"/>
+      <c r="F13" s="113"/>
+      <c r="G13" s="113"/>
+      <c r="H13" s="113"/>
+      <c r="I13" s="113"/>
+      <c r="J13" s="113"/>
+      <c r="K13" s="113"/>
+      <c r="L13" s="113"/>
+      <c r="M13" s="113"/>
+      <c r="N13" s="113"/>
+      <c r="O13" s="113"/>
+      <c r="P13" s="113"/>
+      <c r="Q13" s="113"/>
+      <c r="R13" s="113"/>
+      <c r="S13" s="113"/>
+      <c r="T13" s="113"/>
+      <c r="U13" s="113"/>
+      <c r="V13" s="113"/>
+      <c r="W13" s="113"/>
+      <c r="X13" s="113"/>
+      <c r="Y13" s="128"/>
+      <c r="Z13" s="125"/>
     </row>
     <row r="14" spans="1:26" ht="16.600000000000001" customHeight="1">
       <c r="A14" s="111"/>
-      <c r="B14" s="121"/>
-      <c r="C14" s="120"/>
-      <c r="D14" s="120"/>
-      <c r="E14" s="120"/>
-      <c r="F14" s="120"/>
-      <c r="G14" s="120"/>
-      <c r="H14" s="120"/>
-      <c r="I14" s="120"/>
-      <c r="J14" s="120"/>
-      <c r="K14" s="120"/>
-      <c r="L14" s="120"/>
-      <c r="M14" s="120"/>
-      <c r="N14" s="120"/>
-      <c r="O14" s="120"/>
-      <c r="P14" s="120"/>
-      <c r="Q14" s="120"/>
-      <c r="R14" s="120"/>
-      <c r="S14" s="120"/>
-      <c r="T14" s="120"/>
-      <c r="U14" s="120"/>
-      <c r="V14" s="120"/>
-      <c r="W14" s="120"/>
-      <c r="X14" s="120"/>
-      <c r="Y14" s="135"/>
-      <c r="Z14" s="132"/>
+      <c r="B14" s="114"/>
+      <c r="C14" s="113"/>
+      <c r="D14" s="113"/>
+      <c r="E14" s="113"/>
+      <c r="F14" s="113"/>
+      <c r="G14" s="113"/>
+      <c r="H14" s="113"/>
+      <c r="I14" s="113"/>
+      <c r="J14" s="113"/>
+      <c r="K14" s="113"/>
+      <c r="L14" s="113"/>
+      <c r="M14" s="113"/>
+      <c r="N14" s="113"/>
+      <c r="O14" s="113"/>
+      <c r="P14" s="113"/>
+      <c r="Q14" s="113"/>
+      <c r="R14" s="113"/>
+      <c r="S14" s="113"/>
+      <c r="T14" s="113"/>
+      <c r="U14" s="113"/>
+      <c r="V14" s="113"/>
+      <c r="W14" s="113"/>
+      <c r="X14" s="113"/>
+      <c r="Y14" s="128"/>
+      <c r="Z14" s="125"/>
     </row>
     <row r="15" spans="1:26" ht="16.600000000000001" customHeight="1">
       <c r="A15" s="111"/>
-      <c r="B15" s="121"/>
-      <c r="C15" s="120"/>
-      <c r="D15" s="120"/>
-      <c r="E15" s="120"/>
-      <c r="F15" s="120"/>
-      <c r="G15" s="120"/>
-      <c r="H15" s="120"/>
-      <c r="I15" s="120"/>
-      <c r="J15" s="120"/>
-      <c r="K15" s="120"/>
-      <c r="L15" s="120"/>
-      <c r="M15" s="120"/>
-      <c r="N15" s="120"/>
-      <c r="O15" s="120"/>
-      <c r="P15" s="120"/>
-      <c r="Q15" s="120"/>
-      <c r="R15" s="120"/>
-      <c r="S15" s="120"/>
-      <c r="T15" s="120"/>
-      <c r="U15" s="120"/>
-      <c r="V15" s="120"/>
-      <c r="W15" s="120"/>
-      <c r="X15" s="120"/>
-      <c r="Y15" s="135"/>
-      <c r="Z15" s="132"/>
+      <c r="B15" s="114"/>
+      <c r="C15" s="113"/>
+      <c r="D15" s="113"/>
+      <c r="E15" s="113"/>
+      <c r="F15" s="113"/>
+      <c r="G15" s="113"/>
+      <c r="H15" s="113"/>
+      <c r="I15" s="113"/>
+      <c r="J15" s="113"/>
+      <c r="K15" s="113"/>
+      <c r="L15" s="113"/>
+      <c r="M15" s="113"/>
+      <c r="N15" s="113"/>
+      <c r="O15" s="113"/>
+      <c r="P15" s="113"/>
+      <c r="Q15" s="113"/>
+      <c r="R15" s="113"/>
+      <c r="S15" s="113"/>
+      <c r="T15" s="113"/>
+      <c r="U15" s="113"/>
+      <c r="V15" s="113"/>
+      <c r="W15" s="113"/>
+      <c r="X15" s="113"/>
+      <c r="Y15" s="128"/>
+      <c r="Z15" s="125"/>
     </row>
     <row r="16" spans="1:26" ht="16.600000000000001" customHeight="1">
       <c r="A16" s="111"/>
-      <c r="B16" s="121"/>
-      <c r="C16" s="120"/>
-      <c r="D16" s="120"/>
-      <c r="E16" s="120"/>
-      <c r="F16" s="120"/>
-      <c r="G16" s="120"/>
-      <c r="H16" s="120"/>
-      <c r="I16" s="120"/>
-      <c r="J16" s="120"/>
-      <c r="K16" s="120"/>
-      <c r="L16" s="120"/>
-      <c r="M16" s="120"/>
-      <c r="N16" s="120"/>
-      <c r="O16" s="120"/>
-      <c r="P16" s="120"/>
-      <c r="Q16" s="120"/>
-      <c r="R16" s="120"/>
-      <c r="S16" s="120"/>
-      <c r="T16" s="120"/>
-      <c r="U16" s="120"/>
-      <c r="V16" s="120"/>
-      <c r="W16" s="120"/>
-      <c r="X16" s="120"/>
-      <c r="Y16" s="135"/>
-      <c r="Z16" s="132"/>
+      <c r="B16" s="114"/>
+      <c r="C16" s="113"/>
+      <c r="D16" s="113"/>
+      <c r="E16" s="113"/>
+      <c r="F16" s="113"/>
+      <c r="G16" s="113"/>
+      <c r="H16" s="113"/>
+      <c r="I16" s="113"/>
+      <c r="J16" s="113"/>
+      <c r="K16" s="113"/>
+      <c r="L16" s="113"/>
+      <c r="M16" s="113"/>
+      <c r="N16" s="113"/>
+      <c r="O16" s="113"/>
+      <c r="P16" s="113"/>
+      <c r="Q16" s="113"/>
+      <c r="R16" s="113"/>
+      <c r="S16" s="113"/>
+      <c r="T16" s="113"/>
+      <c r="U16" s="113"/>
+      <c r="V16" s="113"/>
+      <c r="W16" s="113"/>
+      <c r="X16" s="113"/>
+      <c r="Y16" s="128"/>
+      <c r="Z16" s="125"/>
     </row>
     <row r="17" spans="1:26 16384:16384" ht="16.600000000000001" customHeight="1">
       <c r="A17" s="111"/>
-      <c r="B17" s="121"/>
-      <c r="C17" s="120"/>
-      <c r="D17" s="120"/>
-      <c r="E17" s="120"/>
-      <c r="F17" s="120"/>
-      <c r="G17" s="120"/>
-      <c r="H17" s="120"/>
-      <c r="I17" s="120"/>
-      <c r="J17" s="120"/>
-      <c r="K17" s="120"/>
-      <c r="L17" s="120"/>
-      <c r="M17" s="120"/>
-      <c r="N17" s="120"/>
-      <c r="O17" s="120"/>
-      <c r="P17" s="120"/>
-      <c r="Q17" s="120"/>
-      <c r="R17" s="120"/>
-      <c r="S17" s="120"/>
-      <c r="T17" s="120"/>
-      <c r="U17" s="120"/>
-      <c r="V17" s="120"/>
-      <c r="W17" s="120"/>
-      <c r="X17" s="120"/>
-      <c r="Y17" s="135"/>
-      <c r="Z17" s="132"/>
+      <c r="B17" s="114"/>
+      <c r="C17" s="113"/>
+      <c r="D17" s="113"/>
+      <c r="E17" s="113"/>
+      <c r="F17" s="113"/>
+      <c r="G17" s="113"/>
+      <c r="H17" s="113"/>
+      <c r="I17" s="113"/>
+      <c r="J17" s="113"/>
+      <c r="K17" s="113"/>
+      <c r="L17" s="113"/>
+      <c r="M17" s="113"/>
+      <c r="N17" s="113"/>
+      <c r="O17" s="113"/>
+      <c r="P17" s="113"/>
+      <c r="Q17" s="113"/>
+      <c r="R17" s="113"/>
+      <c r="S17" s="113"/>
+      <c r="T17" s="113"/>
+      <c r="U17" s="113"/>
+      <c r="V17" s="113"/>
+      <c r="W17" s="113"/>
+      <c r="X17" s="113"/>
+      <c r="Y17" s="128"/>
+      <c r="Z17" s="125"/>
     </row>
     <row r="18" spans="1:26 16384:16384" ht="16.600000000000001" customHeight="1">
       <c r="A18" s="111"/>
-      <c r="B18" s="121"/>
-      <c r="C18" s="120"/>
-      <c r="D18" s="120"/>
-      <c r="E18" s="120"/>
-      <c r="F18" s="120"/>
-      <c r="G18" s="120"/>
-      <c r="H18" s="120"/>
-      <c r="I18" s="120"/>
-      <c r="J18" s="120"/>
-      <c r="K18" s="120"/>
-      <c r="L18" s="120"/>
-      <c r="M18" s="120"/>
-      <c r="N18" s="120"/>
-      <c r="O18" s="120"/>
-      <c r="P18" s="120"/>
-      <c r="Q18" s="120"/>
-      <c r="R18" s="120"/>
-      <c r="S18" s="120"/>
-      <c r="T18" s="120"/>
-      <c r="U18" s="120"/>
-      <c r="V18" s="120"/>
-      <c r="W18" s="120"/>
-      <c r="X18" s="120"/>
-      <c r="Y18" s="135"/>
-      <c r="Z18" s="132"/>
+      <c r="B18" s="114"/>
+      <c r="C18" s="113"/>
+      <c r="D18" s="113"/>
+      <c r="E18" s="113"/>
+      <c r="F18" s="113"/>
+      <c r="G18" s="113"/>
+      <c r="H18" s="113"/>
+      <c r="I18" s="113"/>
+      <c r="J18" s="113"/>
+      <c r="K18" s="113"/>
+      <c r="L18" s="113"/>
+      <c r="M18" s="113"/>
+      <c r="N18" s="113"/>
+      <c r="O18" s="113"/>
+      <c r="P18" s="113"/>
+      <c r="Q18" s="113"/>
+      <c r="R18" s="113"/>
+      <c r="S18" s="113"/>
+      <c r="T18" s="113"/>
+      <c r="U18" s="113"/>
+      <c r="V18" s="113"/>
+      <c r="W18" s="113"/>
+      <c r="X18" s="113"/>
+      <c r="Y18" s="128"/>
+      <c r="Z18" s="125"/>
     </row>
     <row r="19" spans="1:26 16384:16384" ht="16.600000000000001" customHeight="1">
       <c r="A19" s="111"/>
-      <c r="B19" s="121"/>
-      <c r="C19" s="120"/>
-      <c r="D19" s="120"/>
-      <c r="E19" s="120"/>
-      <c r="F19" s="120"/>
-      <c r="G19" s="120"/>
-      <c r="H19" s="120"/>
-      <c r="I19" s="120"/>
-      <c r="J19" s="120"/>
-      <c r="K19" s="120"/>
-      <c r="L19" s="120"/>
-      <c r="M19" s="120"/>
-      <c r="N19" s="120"/>
-      <c r="O19" s="120"/>
-      <c r="P19" s="120"/>
-      <c r="Q19" s="120"/>
-      <c r="R19" s="120"/>
-      <c r="S19" s="120"/>
-      <c r="T19" s="120"/>
-      <c r="U19" s="120"/>
-      <c r="V19" s="120"/>
-      <c r="W19" s="120"/>
-      <c r="X19" s="120"/>
-      <c r="Y19" s="135"/>
-      <c r="Z19" s="132"/>
+      <c r="B19" s="114"/>
+      <c r="C19" s="113"/>
+      <c r="D19" s="113"/>
+      <c r="E19" s="113"/>
+      <c r="F19" s="113"/>
+      <c r="G19" s="113"/>
+      <c r="H19" s="113"/>
+      <c r="I19" s="113"/>
+      <c r="J19" s="113"/>
+      <c r="K19" s="113"/>
+      <c r="L19" s="113"/>
+      <c r="M19" s="113"/>
+      <c r="N19" s="113"/>
+      <c r="O19" s="113"/>
+      <c r="P19" s="113"/>
+      <c r="Q19" s="113"/>
+      <c r="R19" s="113"/>
+      <c r="S19" s="113"/>
+      <c r="T19" s="113"/>
+      <c r="U19" s="113"/>
+      <c r="V19" s="113"/>
+      <c r="W19" s="113"/>
+      <c r="X19" s="113"/>
+      <c r="Y19" s="128"/>
+      <c r="Z19" s="125"/>
     </row>
     <row r="20" spans="1:26 16384:16384" ht="16.600000000000001" customHeight="1">
       <c r="A20" s="111"/>
-      <c r="B20" s="121"/>
-      <c r="C20" s="120"/>
-      <c r="D20" s="120"/>
-      <c r="E20" s="120"/>
-      <c r="F20" s="120"/>
-      <c r="G20" s="120"/>
-      <c r="H20" s="120"/>
-      <c r="I20" s="120"/>
-      <c r="J20" s="120"/>
-      <c r="K20" s="120"/>
-      <c r="L20" s="120"/>
-      <c r="M20" s="120"/>
-      <c r="N20" s="120"/>
-      <c r="O20" s="120"/>
-      <c r="P20" s="120"/>
-      <c r="Q20" s="120"/>
-      <c r="R20" s="120"/>
-      <c r="S20" s="120"/>
-      <c r="T20" s="120"/>
-      <c r="U20" s="120"/>
-      <c r="V20" s="120"/>
-      <c r="W20" s="120"/>
-      <c r="X20" s="120"/>
-      <c r="Y20" s="135"/>
-      <c r="Z20" s="132"/>
+      <c r="B20" s="114"/>
+      <c r="C20" s="113"/>
+      <c r="D20" s="113"/>
+      <c r="E20" s="113"/>
+      <c r="F20" s="113"/>
+      <c r="G20" s="113"/>
+      <c r="H20" s="113"/>
+      <c r="I20" s="113"/>
+      <c r="J20" s="113"/>
+      <c r="K20" s="113"/>
+      <c r="L20" s="113"/>
+      <c r="M20" s="113"/>
+      <c r="N20" s="113"/>
+      <c r="O20" s="113"/>
+      <c r="P20" s="113"/>
+      <c r="Q20" s="113"/>
+      <c r="R20" s="113"/>
+      <c r="S20" s="113"/>
+      <c r="T20" s="113"/>
+      <c r="U20" s="113"/>
+      <c r="V20" s="113"/>
+      <c r="W20" s="113"/>
+      <c r="X20" s="113"/>
+      <c r="Y20" s="128"/>
+      <c r="Z20" s="125"/>
     </row>
     <row r="21" spans="1:26 16384:16384" ht="16.600000000000001" customHeight="1">
       <c r="A21" s="111"/>
-      <c r="B21" s="121"/>
-      <c r="C21" s="120"/>
-      <c r="D21" s="120"/>
-      <c r="E21" s="120"/>
-      <c r="F21" s="120"/>
-      <c r="G21" s="120"/>
-      <c r="H21" s="120"/>
-      <c r="I21" s="120"/>
-      <c r="J21" s="120"/>
-      <c r="K21" s="120"/>
-      <c r="L21" s="120"/>
-      <c r="M21" s="120"/>
-      <c r="N21" s="120"/>
-      <c r="O21" s="120"/>
-      <c r="P21" s="120"/>
-      <c r="Q21" s="120"/>
-      <c r="R21" s="120"/>
-      <c r="S21" s="120"/>
-      <c r="T21" s="120"/>
-      <c r="U21" s="120"/>
-      <c r="V21" s="120"/>
-      <c r="W21" s="120"/>
-      <c r="X21" s="120"/>
-      <c r="Y21" s="135"/>
-      <c r="Z21" s="132"/>
+      <c r="B21" s="114"/>
+      <c r="C21" s="113"/>
+      <c r="D21" s="113"/>
+      <c r="E21" s="113"/>
+      <c r="F21" s="113"/>
+      <c r="G21" s="113"/>
+      <c r="H21" s="113"/>
+      <c r="I21" s="113"/>
+      <c r="J21" s="113"/>
+      <c r="K21" s="113"/>
+      <c r="L21" s="113"/>
+      <c r="M21" s="113"/>
+      <c r="N21" s="113"/>
+      <c r="O21" s="113"/>
+      <c r="P21" s="113"/>
+      <c r="Q21" s="113"/>
+      <c r="R21" s="113"/>
+      <c r="S21" s="113"/>
+      <c r="T21" s="113"/>
+      <c r="U21" s="113"/>
+      <c r="V21" s="113"/>
+      <c r="W21" s="113"/>
+      <c r="X21" s="113"/>
+      <c r="Y21" s="128"/>
+      <c r="Z21" s="125"/>
     </row>
     <row r="22" spans="1:26 16384:16384" ht="16.600000000000001" customHeight="1">
       <c r="A22" s="111"/>
-      <c r="B22" s="121"/>
-      <c r="C22" s="120"/>
-      <c r="D22" s="120"/>
-      <c r="E22" s="120"/>
-      <c r="F22" s="120"/>
-      <c r="G22" s="120"/>
-      <c r="H22" s="120"/>
-      <c r="I22" s="120"/>
-      <c r="J22" s="120"/>
-      <c r="K22" s="120"/>
-      <c r="L22" s="120"/>
-      <c r="M22" s="120"/>
-      <c r="N22" s="120"/>
-      <c r="O22" s="120"/>
-      <c r="P22" s="120"/>
-      <c r="Q22" s="120"/>
-      <c r="R22" s="120"/>
-      <c r="S22" s="120"/>
-      <c r="T22" s="120"/>
-      <c r="U22" s="120"/>
-      <c r="V22" s="120"/>
-      <c r="W22" s="120"/>
-      <c r="X22" s="120"/>
-      <c r="Y22" s="135"/>
-      <c r="Z22" s="132"/>
+      <c r="B22" s="114"/>
+      <c r="C22" s="113"/>
+      <c r="D22" s="113"/>
+      <c r="E22" s="113"/>
+      <c r="F22" s="113"/>
+      <c r="G22" s="113"/>
+      <c r="H22" s="113"/>
+      <c r="I22" s="113"/>
+      <c r="J22" s="113"/>
+      <c r="K22" s="113"/>
+      <c r="L22" s="113"/>
+      <c r="M22" s="113"/>
+      <c r="N22" s="113"/>
+      <c r="O22" s="113"/>
+      <c r="P22" s="113"/>
+      <c r="Q22" s="113"/>
+      <c r="R22" s="113"/>
+      <c r="S22" s="113"/>
+      <c r="T22" s="113"/>
+      <c r="U22" s="113"/>
+      <c r="V22" s="113"/>
+      <c r="W22" s="113"/>
+      <c r="X22" s="113"/>
+      <c r="Y22" s="128"/>
+      <c r="Z22" s="125"/>
     </row>
     <row r="23" spans="1:26 16384:16384" ht="16.600000000000001" customHeight="1">
       <c r="A23" s="111"/>
-      <c r="B23" s="121"/>
-      <c r="C23" s="120"/>
-      <c r="D23" s="120"/>
-      <c r="E23" s="120"/>
-      <c r="F23" s="120"/>
-      <c r="G23" s="120"/>
-      <c r="H23" s="120"/>
-      <c r="I23" s="120"/>
-      <c r="J23" s="120"/>
-      <c r="K23" s="120"/>
-      <c r="L23" s="120"/>
-      <c r="M23" s="120"/>
-      <c r="N23" s="120"/>
-      <c r="O23" s="120"/>
-      <c r="P23" s="120"/>
-      <c r="Q23" s="120"/>
-      <c r="R23" s="120"/>
-      <c r="S23" s="120"/>
-      <c r="T23" s="120"/>
-      <c r="U23" s="120"/>
-      <c r="V23" s="120"/>
-      <c r="W23" s="120"/>
-      <c r="X23" s="120"/>
-      <c r="Y23" s="135"/>
-      <c r="Z23" s="132"/>
+      <c r="B23" s="114"/>
+      <c r="C23" s="113"/>
+      <c r="D23" s="113"/>
+      <c r="E23" s="113"/>
+      <c r="F23" s="113"/>
+      <c r="G23" s="113"/>
+      <c r="H23" s="113"/>
+      <c r="I23" s="113"/>
+      <c r="J23" s="113"/>
+      <c r="K23" s="113"/>
+      <c r="L23" s="113"/>
+      <c r="M23" s="113"/>
+      <c r="N23" s="113"/>
+      <c r="O23" s="113"/>
+      <c r="P23" s="113"/>
+      <c r="Q23" s="113"/>
+      <c r="R23" s="113"/>
+      <c r="S23" s="113"/>
+      <c r="T23" s="113"/>
+      <c r="U23" s="113"/>
+      <c r="V23" s="113"/>
+      <c r="W23" s="113"/>
+      <c r="X23" s="113"/>
+      <c r="Y23" s="128"/>
+      <c r="Z23" s="125"/>
     </row>
     <row r="24" spans="1:26 16384:16384" ht="16.600000000000001" customHeight="1">
       <c r="A24" s="111"/>
-      <c r="B24" s="121"/>
-      <c r="C24" s="120"/>
-      <c r="D24" s="120"/>
-      <c r="E24" s="120"/>
-      <c r="F24" s="120"/>
-      <c r="G24" s="120"/>
-      <c r="H24" s="120"/>
-      <c r="I24" s="120"/>
-      <c r="J24" s="120"/>
-      <c r="K24" s="120"/>
-      <c r="L24" s="120"/>
-      <c r="M24" s="120"/>
-      <c r="N24" s="120"/>
-      <c r="O24" s="120"/>
-      <c r="P24" s="120"/>
-      <c r="Q24" s="120"/>
-      <c r="R24" s="120"/>
-      <c r="S24" s="120"/>
-      <c r="T24" s="120"/>
-      <c r="U24" s="120"/>
-      <c r="V24" s="120"/>
-      <c r="W24" s="120"/>
-      <c r="X24" s="120"/>
-      <c r="Y24" s="135"/>
-      <c r="Z24" s="132"/>
+      <c r="B24" s="114"/>
+      <c r="C24" s="113"/>
+      <c r="D24" s="113"/>
+      <c r="E24" s="113"/>
+      <c r="F24" s="113"/>
+      <c r="G24" s="113"/>
+      <c r="H24" s="113"/>
+      <c r="I24" s="113"/>
+      <c r="J24" s="113"/>
+      <c r="K24" s="113"/>
+      <c r="L24" s="113"/>
+      <c r="M24" s="113"/>
+      <c r="N24" s="113"/>
+      <c r="O24" s="113"/>
+      <c r="P24" s="113"/>
+      <c r="Q24" s="113"/>
+      <c r="R24" s="113"/>
+      <c r="S24" s="113"/>
+      <c r="T24" s="113"/>
+      <c r="U24" s="113"/>
+      <c r="V24" s="113"/>
+      <c r="W24" s="113"/>
+      <c r="X24" s="113"/>
+      <c r="Y24" s="128"/>
+      <c r="Z24" s="125"/>
     </row>
     <row r="25" spans="1:26 16384:16384" ht="14.65" customHeight="1">
       <c r="A25" s="111"/>
-      <c r="B25" s="121"/>
-      <c r="C25" s="120"/>
-      <c r="D25" s="120"/>
-      <c r="E25" s="120"/>
-      <c r="F25" s="120"/>
-      <c r="G25" s="120"/>
-      <c r="H25" s="120"/>
-      <c r="I25" s="120"/>
-      <c r="J25" s="120"/>
-      <c r="K25" s="120"/>
-      <c r="L25" s="120"/>
-      <c r="M25" s="120"/>
-      <c r="N25" s="120"/>
-      <c r="O25" s="120"/>
-      <c r="P25" s="120"/>
-      <c r="Q25" s="120"/>
-      <c r="R25" s="120"/>
-      <c r="S25" s="120"/>
-      <c r="T25" s="120"/>
-      <c r="U25" s="120"/>
-      <c r="V25" s="120"/>
-      <c r="W25" s="120"/>
-      <c r="X25" s="120"/>
-      <c r="Y25" s="135"/>
-      <c r="Z25" s="132"/>
+      <c r="B25" s="114"/>
+      <c r="C25" s="113"/>
+      <c r="D25" s="113"/>
+      <c r="E25" s="113"/>
+      <c r="F25" s="113"/>
+      <c r="G25" s="113"/>
+      <c r="H25" s="113"/>
+      <c r="I25" s="113"/>
+      <c r="J25" s="113"/>
+      <c r="K25" s="113"/>
+      <c r="L25" s="113"/>
+      <c r="M25" s="113"/>
+      <c r="N25" s="113"/>
+      <c r="O25" s="113"/>
+      <c r="P25" s="113"/>
+      <c r="Q25" s="113"/>
+      <c r="R25" s="113"/>
+      <c r="S25" s="113"/>
+      <c r="T25" s="113"/>
+      <c r="U25" s="113"/>
+      <c r="V25" s="113"/>
+      <c r="W25" s="113"/>
+      <c r="X25" s="113"/>
+      <c r="Y25" s="128"/>
+      <c r="Z25" s="125"/>
     </row>
     <row r="26" spans="1:26 16384:16384" ht="14.65" customHeight="1">
       <c r="A26" s="111"/>
-      <c r="B26" s="121"/>
-      <c r="C26" s="120"/>
-      <c r="D26" s="120"/>
-      <c r="E26" s="120"/>
-      <c r="F26" s="120"/>
-      <c r="G26" s="120"/>
-      <c r="H26" s="120"/>
-      <c r="I26" s="120"/>
-      <c r="J26" s="120"/>
-      <c r="K26" s="120"/>
-      <c r="L26" s="120"/>
-      <c r="M26" s="120"/>
-      <c r="N26" s="120"/>
-      <c r="O26" s="120"/>
-      <c r="P26" s="120"/>
-      <c r="Q26" s="120"/>
-      <c r="R26" s="120"/>
-      <c r="S26" s="120"/>
-      <c r="T26" s="120"/>
-      <c r="U26" s="120"/>
-      <c r="V26" s="120"/>
-      <c r="W26" s="120"/>
-      <c r="X26" s="120"/>
-      <c r="Y26" s="135"/>
-      <c r="Z26" s="132"/>
+      <c r="B26" s="114"/>
+      <c r="C26" s="113"/>
+      <c r="D26" s="113"/>
+      <c r="E26" s="113"/>
+      <c r="F26" s="113"/>
+      <c r="G26" s="113"/>
+      <c r="H26" s="113"/>
+      <c r="I26" s="113"/>
+      <c r="J26" s="113"/>
+      <c r="K26" s="113"/>
+      <c r="L26" s="113"/>
+      <c r="M26" s="113"/>
+      <c r="N26" s="113"/>
+      <c r="O26" s="113"/>
+      <c r="P26" s="113"/>
+      <c r="Q26" s="113"/>
+      <c r="R26" s="113"/>
+      <c r="S26" s="113"/>
+      <c r="T26" s="113"/>
+      <c r="U26" s="113"/>
+      <c r="V26" s="113"/>
+      <c r="W26" s="113"/>
+      <c r="X26" s="113"/>
+      <c r="Y26" s="128"/>
+      <c r="Z26" s="125"/>
     </row>
     <row r="27" spans="1:26 16384:16384" ht="14.65" customHeight="1">
       <c r="A27" s="111"/>
-      <c r="B27" s="121"/>
-      <c r="C27" s="120"/>
-      <c r="D27" s="120"/>
-      <c r="E27" s="120"/>
-      <c r="F27" s="120"/>
-      <c r="G27" s="120"/>
-      <c r="H27" s="120"/>
-      <c r="I27" s="120"/>
-      <c r="J27" s="120"/>
-      <c r="K27" s="120"/>
-      <c r="L27" s="120"/>
-      <c r="M27" s="120"/>
-      <c r="N27" s="120"/>
-      <c r="O27" s="120"/>
-      <c r="P27" s="120"/>
-      <c r="Q27" s="120"/>
-      <c r="R27" s="120"/>
-      <c r="S27" s="120"/>
-      <c r="T27" s="120"/>
-      <c r="U27" s="120"/>
-      <c r="V27" s="120"/>
-      <c r="W27" s="120"/>
-      <c r="X27" s="120"/>
-      <c r="Y27" s="135"/>
-      <c r="Z27" s="132"/>
+      <c r="B27" s="114"/>
+      <c r="C27" s="113"/>
+      <c r="D27" s="113"/>
+      <c r="E27" s="113"/>
+      <c r="F27" s="113"/>
+      <c r="G27" s="113"/>
+      <c r="H27" s="113"/>
+      <c r="I27" s="113"/>
+      <c r="J27" s="113"/>
+      <c r="K27" s="113"/>
+      <c r="L27" s="113"/>
+      <c r="M27" s="113"/>
+      <c r="N27" s="113"/>
+      <c r="O27" s="113"/>
+      <c r="P27" s="113"/>
+      <c r="Q27" s="113"/>
+      <c r="R27" s="113"/>
+      <c r="S27" s="113"/>
+      <c r="T27" s="113"/>
+      <c r="U27" s="113"/>
+      <c r="V27" s="113"/>
+      <c r="W27" s="113"/>
+      <c r="X27" s="113"/>
+      <c r="Y27" s="128"/>
+      <c r="Z27" s="125"/>
     </row>
     <row r="28" spans="1:26 16384:16384" ht="14.65" customHeight="1">
       <c r="A28" s="111"/>
-      <c r="B28" s="121"/>
-      <c r="C28" s="120"/>
-      <c r="D28" s="120"/>
-      <c r="E28" s="120"/>
-      <c r="F28" s="120"/>
-      <c r="G28" s="120"/>
-      <c r="H28" s="120"/>
-      <c r="I28" s="120"/>
-      <c r="J28" s="120"/>
-      <c r="K28" s="120"/>
-      <c r="L28" s="120"/>
-      <c r="M28" s="120"/>
-      <c r="N28" s="120"/>
-      <c r="O28" s="120"/>
-      <c r="P28" s="120"/>
-      <c r="Q28" s="120"/>
-      <c r="R28" s="120"/>
-      <c r="S28" s="120"/>
-      <c r="T28" s="120"/>
-      <c r="U28" s="120"/>
-      <c r="V28" s="120"/>
-      <c r="W28" s="120"/>
-      <c r="X28" s="120"/>
-      <c r="Y28" s="135"/>
-      <c r="Z28" s="132"/>
+      <c r="B28" s="114"/>
+      <c r="C28" s="113"/>
+      <c r="D28" s="113"/>
+      <c r="E28" s="113"/>
+      <c r="F28" s="113"/>
+      <c r="G28" s="113"/>
+      <c r="H28" s="113"/>
+      <c r="I28" s="113"/>
+      <c r="J28" s="113"/>
+      <c r="K28" s="113"/>
+      <c r="L28" s="113"/>
+      <c r="M28" s="113"/>
+      <c r="N28" s="113"/>
+      <c r="O28" s="113"/>
+      <c r="P28" s="113"/>
+      <c r="Q28" s="113"/>
+      <c r="R28" s="113"/>
+      <c r="S28" s="113"/>
+      <c r="T28" s="113"/>
+      <c r="U28" s="113"/>
+      <c r="V28" s="113"/>
+      <c r="W28" s="113"/>
+      <c r="X28" s="113"/>
+      <c r="Y28" s="128"/>
+      <c r="Z28" s="125"/>
     </row>
     <row r="29" spans="1:26 16384:16384" ht="14.65" customHeight="1">
       <c r="A29" s="111"/>
-      <c r="B29" s="121"/>
-      <c r="C29" s="120"/>
-      <c r="D29" s="120"/>
-      <c r="E29" s="120"/>
-      <c r="F29" s="120"/>
-      <c r="G29" s="120"/>
-      <c r="H29" s="120"/>
-      <c r="I29" s="120"/>
-      <c r="J29" s="120"/>
-      <c r="K29" s="120"/>
-      <c r="L29" s="120"/>
-      <c r="M29" s="120"/>
-      <c r="N29" s="120"/>
-      <c r="O29" s="120"/>
-      <c r="P29" s="120"/>
-      <c r="Q29" s="120"/>
-      <c r="R29" s="120"/>
-      <c r="S29" s="120"/>
-      <c r="T29" s="120"/>
-      <c r="U29" s="120"/>
-      <c r="V29" s="120"/>
-      <c r="W29" s="120"/>
-      <c r="X29" s="120"/>
-      <c r="Y29" s="135"/>
-      <c r="Z29" s="132"/>
+      <c r="B29" s="114"/>
+      <c r="C29" s="113"/>
+      <c r="D29" s="113"/>
+      <c r="E29" s="113"/>
+      <c r="F29" s="113"/>
+      <c r="G29" s="113"/>
+      <c r="H29" s="113"/>
+      <c r="I29" s="113"/>
+      <c r="J29" s="113"/>
+      <c r="K29" s="113"/>
+      <c r="L29" s="113"/>
+      <c r="M29" s="113"/>
+      <c r="N29" s="113"/>
+      <c r="O29" s="113"/>
+      <c r="P29" s="113"/>
+      <c r="Q29" s="113"/>
+      <c r="R29" s="113"/>
+      <c r="S29" s="113"/>
+      <c r="T29" s="113"/>
+      <c r="U29" s="113"/>
+      <c r="V29" s="113"/>
+      <c r="W29" s="113"/>
+      <c r="X29" s="113"/>
+      <c r="Y29" s="128"/>
+      <c r="Z29" s="125"/>
     </row>
     <row r="30" spans="1:26 16384:16384" ht="14.65" customHeight="1">
       <c r="A30" s="111"/>
-      <c r="B30" s="121"/>
-      <c r="C30" s="120"/>
-      <c r="D30" s="120"/>
-      <c r="E30" s="120"/>
-      <c r="F30" s="120"/>
-      <c r="G30" s="120"/>
-      <c r="H30" s="120"/>
-      <c r="I30" s="120"/>
-      <c r="J30" s="120"/>
-      <c r="K30" s="120"/>
-      <c r="L30" s="120"/>
-      <c r="M30" s="120"/>
-      <c r="N30" s="120"/>
-      <c r="O30" s="120"/>
-      <c r="P30" s="120"/>
-      <c r="Q30" s="120"/>
-      <c r="R30" s="120"/>
-      <c r="S30" s="120"/>
-      <c r="T30" s="120"/>
-      <c r="U30" s="120"/>
-      <c r="V30" s="120"/>
-      <c r="W30" s="120"/>
-      <c r="X30" s="120"/>
-      <c r="Y30" s="135"/>
-      <c r="Z30" s="132"/>
+      <c r="B30" s="114"/>
+      <c r="C30" s="113"/>
+      <c r="D30" s="113"/>
+      <c r="E30" s="113"/>
+      <c r="F30" s="113"/>
+      <c r="G30" s="113"/>
+      <c r="H30" s="113"/>
+      <c r="I30" s="113"/>
+      <c r="J30" s="113"/>
+      <c r="K30" s="113"/>
+      <c r="L30" s="113"/>
+      <c r="M30" s="113"/>
+      <c r="N30" s="113"/>
+      <c r="O30" s="113"/>
+      <c r="P30" s="113"/>
+      <c r="Q30" s="113"/>
+      <c r="R30" s="113"/>
+      <c r="S30" s="113"/>
+      <c r="T30" s="113"/>
+      <c r="U30" s="113"/>
+      <c r="V30" s="113"/>
+      <c r="W30" s="113"/>
+      <c r="X30" s="113"/>
+      <c r="Y30" s="128"/>
+      <c r="Z30" s="125"/>
     </row>
     <row r="31" spans="1:26 16384:16384" ht="14.65" customHeight="1">
       <c r="A31" s="111"/>
-      <c r="B31" s="120"/>
-      <c r="C31" s="120"/>
-      <c r="D31" s="120"/>
-      <c r="E31" s="120"/>
-      <c r="F31" s="120"/>
-      <c r="G31" s="120"/>
-      <c r="H31" s="120"/>
-      <c r="I31" s="120"/>
-      <c r="J31" s="120"/>
-      <c r="K31" s="120"/>
-      <c r="L31" s="120"/>
-      <c r="M31" s="120"/>
-      <c r="N31" s="120"/>
-      <c r="O31" s="120"/>
-      <c r="P31" s="120"/>
-      <c r="Q31" s="120"/>
-      <c r="R31" s="120"/>
-      <c r="S31" s="120"/>
-      <c r="T31" s="120"/>
-      <c r="U31" s="120"/>
-      <c r="V31" s="120"/>
-      <c r="W31" s="120"/>
-      <c r="X31" s="120"/>
-      <c r="Y31" s="135"/>
-      <c r="Z31" s="132"/>
-    </row>
-    <row r="32" spans="1:26 16384:16384" s="129" customFormat="1" ht="14.65" customHeight="1">
-      <c r="A32" s="119"/>
-      <c r="B32" s="122"/>
-      <c r="C32" s="123"/>
-      <c r="D32" s="123"/>
-      <c r="E32" s="123"/>
-      <c r="F32" s="123"/>
-      <c r="G32" s="123"/>
-      <c r="H32" s="123"/>
-      <c r="I32" s="123"/>
-      <c r="J32" s="123"/>
-      <c r="K32" s="123"/>
-      <c r="L32" s="123"/>
-      <c r="M32" s="123"/>
-      <c r="N32" s="123"/>
-      <c r="O32" s="123"/>
-      <c r="P32" s="123"/>
-      <c r="Q32" s="123"/>
-      <c r="R32" s="123"/>
-      <c r="S32" s="123"/>
-      <c r="T32" s="123"/>
-      <c r="U32" s="123"/>
-      <c r="V32" s="123"/>
-      <c r="W32" s="123"/>
-      <c r="X32" s="123"/>
-      <c r="Y32" s="136"/>
-      <c r="Z32" s="133"/>
-      <c r="XFD32" s="139"/>
+      <c r="B31" s="113"/>
+      <c r="C31" s="113"/>
+      <c r="D31" s="113"/>
+      <c r="E31" s="113"/>
+      <c r="F31" s="113"/>
+      <c r="G31" s="113"/>
+      <c r="H31" s="113"/>
+      <c r="I31" s="113"/>
+      <c r="J31" s="113"/>
+      <c r="K31" s="113"/>
+      <c r="L31" s="113"/>
+      <c r="M31" s="113"/>
+      <c r="N31" s="113"/>
+      <c r="O31" s="113"/>
+      <c r="P31" s="113"/>
+      <c r="Q31" s="113"/>
+      <c r="R31" s="113"/>
+      <c r="S31" s="113"/>
+      <c r="T31" s="113"/>
+      <c r="U31" s="113"/>
+      <c r="V31" s="113"/>
+      <c r="W31" s="113"/>
+      <c r="X31" s="113"/>
+      <c r="Y31" s="128"/>
+      <c r="Z31" s="125"/>
+    </row>
+    <row r="32" spans="1:26 16384:16384" s="122" customFormat="1" ht="14.65" customHeight="1">
+      <c r="A32" s="112"/>
+      <c r="B32" s="115"/>
+      <c r="C32" s="116"/>
+      <c r="D32" s="116"/>
+      <c r="E32" s="116"/>
+      <c r="F32" s="116"/>
+      <c r="G32" s="116"/>
+      <c r="H32" s="116"/>
+      <c r="I32" s="116"/>
+      <c r="J32" s="116"/>
+      <c r="K32" s="116"/>
+      <c r="L32" s="116"/>
+      <c r="M32" s="116"/>
+      <c r="N32" s="116"/>
+      <c r="O32" s="116"/>
+      <c r="P32" s="116"/>
+      <c r="Q32" s="116"/>
+      <c r="R32" s="116"/>
+      <c r="S32" s="116"/>
+      <c r="T32" s="116"/>
+      <c r="U32" s="116"/>
+      <c r="V32" s="116"/>
+      <c r="W32" s="116"/>
+      <c r="X32" s="116"/>
+      <c r="Y32" s="129"/>
+      <c r="Z32" s="126"/>
+      <c r="XFD32" s="132"/>
     </row>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="96ymJI72tcrmk4qAUka3T4dwmpdFgkLDlSEJpzyz7mWD7vsWEuXmIL2sUDp1eg9iF8+BlwTgDaTzxaNDJoc1mg==" saltValue="+Es6UJjmwgiP69Amte+fOA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
@@ -12456,10 +11881,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="24" customHeight="1">
-      <c r="A1" s="117" t="s">
+      <c r="A1" s="178" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="118"/>
+      <c r="B1" s="179"/>
       <c r="C1" s="50" t="s">
         <v>78</v>
       </c>
@@ -13167,7 +12592,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:XFD23"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" workbookViewId="0">
       <pane xSplit="2" topLeftCell="F1" activePane="topRight" state="frozen"/>
@@ -13340,7 +12765,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:XFD13"/>
+  <dimension ref="A1:XFC13"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" workbookViewId="0">
       <pane xSplit="6" topLeftCell="G1" activePane="topRight" state="frozen"/>

</xml_diff>